<commit_message>
collated all results and initial thoughts
</commit_message>
<xml_diff>
--- a/Thesis/Code/enron_dynet_attvol.xlsx
+++ b/Thesis/Code/enron_dynet_attvol.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>AvgDeg</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Emergence</t>
+  </si>
+  <si>
+    <t>NormNMFRatio</t>
   </si>
   <si>
     <t>Nov98</t>
@@ -578,13 +581,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z45"/>
+  <dimension ref="A1:AA45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,10 +663,13 @@
       <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0.142857142857143</v>
@@ -675,7 +681,7 @@
         <v>0.125</v>
       </c>
       <c r="E2">
-        <v>0.188611313365478</v>
+        <v>0.222018968604531</v>
       </c>
       <c r="F2">
         <v>0.18543463409279</v>
@@ -690,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="K2">
         <v>-0.196246760424671</v>
@@ -740,10 +746,13 @@
       <c r="Z2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:26">
+      <c r="AA2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0.145454545454545</v>
@@ -755,7 +764,7 @@
         <v>0.0868686868686869</v>
       </c>
       <c r="E3">
-        <v>0.198999299503384</v>
+        <v>0.233759914226578</v>
       </c>
       <c r="F3">
         <v>0.175110542980077</v>
@@ -812,18 +821,21 @@
         <v>-0.310794340746057</v>
       </c>
       <c r="X3">
-        <v>0.798451031971622</v>
+        <v>0.355047508500758</v>
       </c>
       <c r="Y3">
         <v>0.0130686392313725</v>
       </c>
       <c r="Z3">
-        <v>0.433631360458153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
+        <v>0.485409215907839</v>
+      </c>
+      <c r="AA3">
+        <v>1.47806084097062</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0.0833333333333333</v>
@@ -892,18 +904,21 @@
         <v>0.538397982609507</v>
       </c>
       <c r="X4">
-        <v>1.2727005629334</v>
+        <v>1.43726655438487</v>
       </c>
       <c r="Y4">
         <v>0.0157442604741007</v>
       </c>
       <c r="Z4">
-        <v>0.0105686191249875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26">
+        <v>0.0187120544090581</v>
+      </c>
+      <c r="AA4">
+        <v>0.89568857487168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -972,18 +987,21 @@
         <v>-1.05191082665109</v>
       </c>
       <c r="X5">
-        <v>-0.793122030534896</v>
+        <v>-0.682907060830884</v>
       </c>
       <c r="Y5">
         <v>0.00878987146533087</v>
       </c>
       <c r="Z5">
-        <v>-0.117516200256448</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
+        <v>-0.155184651760784</v>
+      </c>
+      <c r="AA5">
+        <v>0.487905759876115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>0.2</v>
@@ -995,7 +1013,7 @@
         <v>0.166666666666667</v>
       </c>
       <c r="E6">
-        <v>0.275965013206177</v>
+        <v>0.32866964087565</v>
       </c>
       <c r="F6">
         <v>0.277684053800249</v>
@@ -1010,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="K6">
         <v>-0.157405383455039</v>
@@ -1052,18 +1070,21 @@
         <v>1.69741990976954</v>
       </c>
       <c r="X6">
-        <v>0.380167937256847</v>
+        <v>0.986995014038095</v>
       </c>
       <c r="Y6">
         <v>0.0124307554377872</v>
       </c>
       <c r="Z6">
-        <v>0.244502312299965</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
+        <v>0.297927735126215</v>
+      </c>
+      <c r="AA6">
+        <v>1.31832895468212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -1090,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>-0.0587497473260579</v>
@@ -1132,18 +1153,21 @@
         <v>-1.69741990976954</v>
       </c>
       <c r="X7">
-        <v>-0.137848567247918</v>
+        <v>-1.19139090968465</v>
       </c>
       <c r="Y7">
         <v>0.0124307554377872</v>
       </c>
       <c r="Z7">
-        <v>-0.196578488289321</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
+        <v>-0.378621196499424</v>
+      </c>
+      <c r="AA7">
+        <v>0.75853602126271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>0.120879120879121</v>
@@ -1212,18 +1236,21 @@
         <v>1.04529271084357</v>
       </c>
       <c r="X8">
-        <v>0.313873826629775</v>
+        <v>0.429239578071182</v>
       </c>
       <c r="Y8">
         <v>0.0070118917343666</v>
       </c>
       <c r="Z8">
-        <v>0.0467810459780721</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+        <v>0.302081121206406</v>
+      </c>
+      <c r="AA8">
+        <v>2.01279597217926</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>0.0661764705882353</v>
@@ -1292,18 +1319,21 @@
         <v>14.0709202030539</v>
       </c>
       <c r="X9">
-        <v>0.71325656118837</v>
+        <v>1.05723215840821</v>
       </c>
       <c r="Y9">
         <v>0.0145159949751711</v>
       </c>
       <c r="Z9">
-        <v>0.557029805131976</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
+        <v>0.48966865698235</v>
+      </c>
+      <c r="AA9">
+        <v>0.908884467951915</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>0.0947712418300654</v>
@@ -1330,7 +1360,7 @@
         <v>0.387962962962963</v>
       </c>
       <c r="J10">
-        <v>0.238465591590028</v>
+        <v>0.238465591590027</v>
       </c>
       <c r="K10">
         <v>-0.176051138447516</v>
@@ -1372,7 +1402,7 @@
         <v>-13.6340352261333</v>
       </c>
       <c r="X10">
-        <v>-1.43569166916603</v>
+        <v>-1.10049676408314</v>
       </c>
       <c r="Y10">
         <v>0.0131379693689775</v>
@@ -1380,10 +1410,13 @@
       <c r="Z10">
         <v>-1</v>
       </c>
-    </row>
-    <row r="11" spans="1:26">
+      <c r="AA10">
+        <v>1.72134344587126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>0.0887445887445887</v>
@@ -1395,7 +1428,7 @@
         <v>0.0571428571428571</v>
       </c>
       <c r="E11">
-        <v>0.140038689430161</v>
+        <v>0.14296285615201</v>
       </c>
       <c r="F11">
         <v>0.183911998623885</v>
@@ -1452,7 +1485,7 @@
         <v>-0.192578685742613</v>
       </c>
       <c r="X11">
-        <v>-0.117858427482473</v>
+        <v>0.333995250421391</v>
       </c>
       <c r="Y11">
         <v>0.0150361523392413</v>
@@ -1460,10 +1493,13 @@
       <c r="Z11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="AA11">
+        <v>0.817432300754284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>0.0711462450592885</v>
@@ -1490,7 +1526,7 @@
         <v>0.311242863416776</v>
       </c>
       <c r="J12">
-        <v>0.159162627197143</v>
+        <v>0.159162627197141</v>
       </c>
       <c r="K12">
         <v>-0.196526804855736</v>
@@ -1532,18 +1568,21 @@
         <v>1.0337269710037</v>
       </c>
       <c r="X12">
-        <v>0.184319057172725</v>
+        <v>-1.01153684225008</v>
       </c>
       <c r="Y12">
         <v>0.0140866989190509</v>
       </c>
       <c r="Z12">
-        <v>0.164630208691889</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
+        <v>0.00625326125694494</v>
+      </c>
+      <c r="AA12">
+        <v>1.22070400001624</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>0.0707692307692308</v>
@@ -1555,7 +1594,7 @@
         <v>0.0288034188034188</v>
       </c>
       <c r="E13">
-        <v>0.136185194327928</v>
+        <v>0.127862044081464</v>
       </c>
       <c r="F13">
         <v>0.17244723549779</v>
@@ -1612,18 +1651,21 @@
         <v>-1.63461113465214</v>
       </c>
       <c r="X13">
-        <v>-0.0369306897351715</v>
+        <v>-0.804111484444151</v>
       </c>
       <c r="Y13">
         <v>0.0154534567266276</v>
       </c>
       <c r="Z13">
-        <v>-0.490671182955242</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26">
+        <v>-0.429681316969979</v>
+      </c>
+      <c r="AA13">
+        <v>1.26845788294828</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>0.0857142857142857</v>
@@ -1692,18 +1734,21 @@
         <v>2.22407908330382</v>
       </c>
       <c r="X14">
-        <v>-0.140603794551299</v>
+        <v>-1.2835483451852</v>
       </c>
       <c r="Y14">
         <v>0.0160828854606541</v>
       </c>
       <c r="Z14">
-        <v>0.561742183885765</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
+        <v>0.499565787028071</v>
+      </c>
+      <c r="AA14">
+        <v>0.603924264107491</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>0.0256892230576441</v>
@@ -1715,7 +1760,7 @@
         <v>0.0388357256778309</v>
       </c>
       <c r="E15">
-        <v>0.0699805257841254</v>
+        <v>0.0696624296349748</v>
       </c>
       <c r="F15">
         <v>0.106213076196652</v>
@@ -1772,18 +1817,21 @@
         <v>0.700871081985116</v>
       </c>
       <c r="X15">
-        <v>-1.24049507302092</v>
+        <v>1.40446799016771</v>
       </c>
       <c r="Y15">
         <v>0.0113929755478287</v>
       </c>
       <c r="Z15">
-        <v>-0.567016618789838</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
+        <v>0.0440367493189775</v>
+      </c>
+      <c r="AA15">
+        <v>3.47512635591994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>0.0223776223776224</v>
@@ -1795,7 +1843,7 @@
         <v>0.0349478126040626</v>
       </c>
       <c r="E16">
-        <v>0.0688937933411225</v>
+        <v>0.0669982594194598</v>
       </c>
       <c r="F16">
         <v>0.0995557405453889</v>
@@ -1852,18 +1900,21 @@
         <v>-2.8331062521871</v>
       </c>
       <c r="X16">
-        <v>0.212114876518291</v>
+        <v>-0.204270994099142</v>
       </c>
       <c r="Y16">
         <v>0.0145604426441847</v>
       </c>
       <c r="Z16">
-        <v>-0.341604863756992</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26">
+        <v>-0.708034937602533</v>
+      </c>
+      <c r="AA16">
+        <v>0.648501521447253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17">
         <v>0.0266257040450589</v>
@@ -1875,7 +1926,7 @@
         <v>0.0353255645051369</v>
       </c>
       <c r="E17">
-        <v>0.083169663428687</v>
+        <v>0.0843351358953168</v>
       </c>
       <c r="F17">
         <v>0.104651531925811</v>
@@ -1932,18 +1983,21 @@
         <v>1.17264436501075</v>
       </c>
       <c r="X17">
-        <v>0.516442976012976</v>
+        <v>-0.277466947794664</v>
       </c>
       <c r="Y17">
         <v>0.014825334134991</v>
       </c>
       <c r="Z17">
-        <v>0.667448602068278</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26">
+        <v>0.672292340219475</v>
+      </c>
+      <c r="AA17">
+        <v>0.986712034676278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18">
         <v>0.014809329877823</v>
@@ -1955,7 +2009,7 @@
         <v>0.0465311201612571</v>
       </c>
       <c r="E18">
-        <v>0.0657119563945911</v>
+        <v>0.0650027797097374</v>
       </c>
       <c r="F18">
         <v>0.0973542790063602</v>
@@ -1970,7 +2024,7 @@
         <v>0.235756360756361</v>
       </c>
       <c r="J18">
-        <v>0.0646489545249861</v>
+        <v>0.0646489545249898</v>
       </c>
       <c r="K18">
         <v>-0.237276142988631</v>
@@ -2012,18 +2066,21 @@
         <v>-0.246935913586076</v>
       </c>
       <c r="X18">
-        <v>0.403708513641944</v>
+        <v>0.134541549332513</v>
       </c>
       <c r="Y18">
         <v>0.0153540765528727</v>
       </c>
       <c r="Z18">
-        <v>-0.240676664210239</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26">
+        <v>-0.201712149724085</v>
+      </c>
+      <c r="AA18">
+        <v>1.15017241711094</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>0.0104642313546423</v>
@@ -2035,7 +2092,7 @@
         <v>0.0422642399296846</v>
       </c>
       <c r="E19">
-        <v>0.053698032906828</v>
+        <v>0.053698032906832</v>
       </c>
       <c r="F19">
         <v>0.103359082534663</v>
@@ -2092,18 +2149,21 @@
         <v>-0.370739975058558</v>
       </c>
       <c r="X19">
-        <v>-1.678232437937</v>
+        <v>-1.3451979492215</v>
       </c>
       <c r="Y19">
         <v>0.0158764726629214</v>
       </c>
       <c r="Z19">
-        <v>0.245745091401968</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26">
+        <v>0.277950671015695</v>
+      </c>
+      <c r="AA19">
+        <v>1.06896439663969</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>0.0140350877192982</v>
@@ -2115,7 +2175,7 @@
         <v>0.0330912754860123</v>
       </c>
       <c r="E20">
-        <v>0.072435091637446</v>
+        <v>0.0714575293344729</v>
       </c>
       <c r="F20">
         <v>0.104187684027673</v>
@@ -2166,24 +2226,27 @@
         <v>3.99088824392554</v>
       </c>
       <c r="V20">
-        <v>0.884417516687753</v>
+        <v>0.884417516687752</v>
       </c>
       <c r="W20">
         <v>1.05075613713745</v>
       </c>
       <c r="X20">
-        <v>1.61210570618281</v>
+        <v>3.61505799642203</v>
       </c>
       <c r="Y20">
         <v>0.0141937749294579</v>
       </c>
       <c r="Z20">
-        <v>-0.163703159323353</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26">
+        <v>0.0472228955487312</v>
+      </c>
+      <c r="AA20">
+        <v>0.907380390841924</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21">
         <v>0.0108669108669109</v>
@@ -2246,24 +2309,27 @@
         <v>3.46593592744942</v>
       </c>
       <c r="V21">
-        <v>0.88358062226478</v>
+        <v>0.883580622264781</v>
       </c>
       <c r="W21">
         <v>1.145740474131</v>
       </c>
       <c r="X21">
-        <v>-1.96649833839107</v>
+        <v>-0.323226998341732</v>
       </c>
       <c r="Y21">
         <v>0.0145117123390032</v>
       </c>
       <c r="Z21">
-        <v>-0.232054467941425</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26">
+        <v>-0.265848917549648</v>
+      </c>
+      <c r="AA21">
+        <v>0.993876622141327</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>0.012697323266987</v>
@@ -2275,7 +2341,7 @@
         <v>0.0267869971306903</v>
       </c>
       <c r="E22">
-        <v>0.0682675509441143</v>
+        <v>0.0683111177551116</v>
       </c>
       <c r="F22">
         <v>0.0860935286033843</v>
@@ -2332,18 +2398,21 @@
         <v>-1.50978661909184</v>
       </c>
       <c r="X22">
-        <v>-0.231105429387745</v>
+        <v>-0.224611224193025</v>
       </c>
       <c r="Y22">
         <v>0.014594047644061</v>
       </c>
       <c r="Z22">
-        <v>0.15471651044799</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26">
+        <v>-0.0177951937566633</v>
+      </c>
+      <c r="AA22">
+        <v>1.14969210902986</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23">
         <v>0.0165137614678899</v>
@@ -2355,7 +2424,7 @@
         <v>0.017814682061624</v>
       </c>
       <c r="E23">
-        <v>0.0627867102642266</v>
+        <v>0.0633610614551491</v>
       </c>
       <c r="F23">
         <v>0.0684365807313087</v>
@@ -2412,18 +2481,21 @@
         <v>1.12579431337031</v>
       </c>
       <c r="X23">
-        <v>-0.589048951470494</v>
+        <v>0.566559629994456</v>
       </c>
       <c r="Y23">
         <v>0.014389861392556</v>
       </c>
       <c r="Z23">
-        <v>-0.375441043150031</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26">
+        <v>-0.190533185638212</v>
+      </c>
+      <c r="AA23">
+        <v>0.823466610119958</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24">
         <v>0.0121474685694869</v>
@@ -2435,7 +2507,7 @@
         <v>0.0194173148347547</v>
       </c>
       <c r="E24">
-        <v>0.0617225746596252</v>
+        <v>0.0620148193059091</v>
       </c>
       <c r="F24">
         <v>0.0737468264816389</v>
@@ -2492,18 +2564,21 @@
         <v>-0.541538212690746</v>
       </c>
       <c r="X24">
-        <v>-0.000614025599084254</v>
+        <v>0.445841546612435</v>
       </c>
       <c r="Y24">
         <v>0.0161524545736765</v>
       </c>
       <c r="Z24">
-        <v>0.125239704335393</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26">
+        <v>0.452650931285279</v>
+      </c>
+      <c r="AA24">
+        <v>6.36640412963768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25">
         <v>0.018085842852198</v>
@@ -2515,7 +2590,7 @@
         <v>0.0197769330858305</v>
       </c>
       <c r="E25">
-        <v>0.0624494123772589</v>
+        <v>0.0625371639735348</v>
       </c>
       <c r="F25">
         <v>0.0641638796808436</v>
@@ -2572,18 +2647,21 @@
         <v>-0.40115131886765</v>
       </c>
       <c r="X25">
-        <v>0.570823866952195</v>
+        <v>-0.0141925663441352</v>
       </c>
       <c r="Y25">
         <v>0.0153914881537371</v>
       </c>
       <c r="Z25">
-        <v>0.128885812910686</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26">
+        <v>-0.568600024615127</v>
+      </c>
+      <c r="AA25">
+        <v>0.158850872775147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B26">
         <v>0.0108838185156045</v>
@@ -2652,18 +2730,21 @@
         <v>0.0650015997574016</v>
       </c>
       <c r="X26">
-        <v>-0.197714809118101</v>
+        <v>-0.301618269630589</v>
       </c>
       <c r="Y26">
         <v>0.0157083458970645</v>
       </c>
       <c r="Z26">
-        <v>-0.18548877317808</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26">
+        <v>0.290270924639705</v>
+      </c>
+      <c r="AA26">
+        <v>2.31070909967728</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B27">
         <v>0.013886910696482</v>
@@ -2675,7 +2756,7 @@
         <v>0.0191988138149654</v>
       </c>
       <c r="E27">
-        <v>0.0514510159016959</v>
+        <v>0.051451015901696</v>
       </c>
       <c r="F27">
         <v>0.0389426665588692</v>
@@ -2732,18 +2813,21 @@
         <v>-0.141684921779725</v>
       </c>
       <c r="X27">
-        <v>1.92946261482969</v>
+        <v>1.70875345594072</v>
       </c>
       <c r="Y27">
         <v>0.0154573970921823</v>
       </c>
       <c r="Z27">
-        <v>0.452563183036544</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26">
+        <v>0.181863517060296</v>
+      </c>
+      <c r="AA27">
+        <v>0.487947303386618</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B28">
         <v>0.0131785995279308</v>
@@ -2812,18 +2896,21 @@
         <v>-0.491368424547045</v>
       </c>
       <c r="X28">
-        <v>0.0585820886219431</v>
+        <v>0.739502362394502</v>
       </c>
       <c r="Y28">
         <v>0.0159509673976893</v>
       </c>
       <c r="Z28">
-        <v>-0.507271960672089</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26">
+        <v>-0.362684784623684</v>
+      </c>
+      <c r="AA28">
+        <v>0.938555672609553</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B29">
         <v>0.0120518688024409</v>
@@ -2835,7 +2922,7 @@
         <v>0.0218669203863541</v>
       </c>
       <c r="E29">
-        <v>0.0649339033932292</v>
+        <v>0.0646855661853243</v>
       </c>
       <c r="F29">
         <v>0.074620180597347</v>
@@ -2892,18 +2979,21 @@
         <v>-0.225297129925138</v>
       </c>
       <c r="X29">
-        <v>-0.228416012619717</v>
+        <v>0.599420682217894</v>
       </c>
       <c r="Y29">
         <v>0.0163705868910213</v>
       </c>
       <c r="Z29">
-        <v>-0.242034924167696</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26">
+        <v>-0.0319605398737786</v>
+      </c>
+      <c r="AA29">
+        <v>1.19335042512633</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B30">
         <v>0.0129819040125885</v>
@@ -2915,7 +3005,7 @@
         <v>0.0175248267621899</v>
       </c>
       <c r="E30">
-        <v>0.0587812459360855</v>
+        <v>0.0587941074784044</v>
       </c>
       <c r="F30">
         <v>0.0573386507422087</v>
@@ -2972,18 +3062,21 @@
         <v>0.227354792574308</v>
       </c>
       <c r="X30">
-        <v>-0.671834809845069</v>
+        <v>0.0888315252844555</v>
       </c>
       <c r="Y30">
         <v>0.0156018477241692</v>
       </c>
       <c r="Z30">
-        <v>0.355304574814682</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26">
+        <v>0.156708865525271</v>
+      </c>
+      <c r="AA30">
+        <v>0.946094252235949</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B31">
         <v>0.0156071998177261</v>
@@ -2995,7 +3088,7 @@
         <v>0.0179282348828351</v>
       </c>
       <c r="E31">
-        <v>0.0517206953879717</v>
+        <v>0.0519141811073833</v>
       </c>
       <c r="F31">
         <v>0.00299546276384042</v>
@@ -3052,18 +3145,21 @@
         <v>1.30380508791649</v>
       </c>
       <c r="X31">
-        <v>-2.0824985294267</v>
+        <v>-2.21678463990497</v>
       </c>
       <c r="Y31">
         <v>0.0155941129759143</v>
       </c>
       <c r="Z31">
-        <v>-0.278886218407177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26">
+        <v>-0.367164455694182</v>
+      </c>
+      <c r="AA31">
+        <v>0.904090206526913</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B32">
         <v>0.0124005027230834</v>
@@ -3075,7 +3171,7 @@
         <v>0.0115482368474337</v>
       </c>
       <c r="E32">
-        <v>0.054498945448189</v>
+        <v>0.0529949940828381</v>
       </c>
       <c r="F32">
         <v>0.0221077853966976</v>
@@ -3132,18 +3228,21 @@
         <v>-0.485540704138178</v>
       </c>
       <c r="X32">
-        <v>-2.70919208784593</v>
+        <v>-0.893012985764048</v>
       </c>
       <c r="Y32">
         <v>0.0155906223665728</v>
       </c>
       <c r="Z32">
-        <v>-0.759617298624853</v>
-      </c>
-    </row>
-    <row r="33" spans="1:26">
+        <v>-0.0246133482319035</v>
+      </c>
+      <c r="AA32">
+        <v>1.05616235065536</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B33">
         <v>0.00881458966565349</v>
@@ -3170,7 +3269,7 @@
         <v>0.326122897076721</v>
       </c>
       <c r="J33">
-        <v>0.149515347706407</v>
+        <v>0.149515347706408</v>
       </c>
       <c r="K33">
         <v>-0.2742315177481</v>
@@ -3212,18 +3311,21 @@
         <v>-0.730432509767316</v>
       </c>
       <c r="X33">
-        <v>1.10696080467523</v>
+        <v>-0.571122678617127</v>
       </c>
       <c r="Y33">
         <v>0.0164239032884816</v>
       </c>
       <c r="Z33">
-        <v>0.913079264504755</v>
-      </c>
-    </row>
-    <row r="34" spans="1:26">
+        <v>0.572047289486678</v>
+      </c>
+      <c r="AA33">
+        <v>0.989825199424454</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B34">
         <v>0.0160364145658263</v>
@@ -3235,7 +3337,7 @@
         <v>0.0205392822254736</v>
       </c>
       <c r="E34">
-        <v>0.0534003926785189</v>
+        <v>0.0536597775812678</v>
       </c>
       <c r="F34">
         <v>0.0465793288516832</v>
@@ -3292,18 +3394,21 @@
         <v>1.41127049960005</v>
       </c>
       <c r="X34">
-        <v>-0.677068670856111</v>
+        <v>1.0709850128508</v>
       </c>
       <c r="Y34">
         <v>0.0144777445925457</v>
       </c>
       <c r="Z34">
-        <v>-0.315395941933631</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26">
+        <v>0.0382293318183974</v>
+      </c>
+      <c r="AA34">
+        <v>0.963061159874462</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B35">
         <v>0.0166390270867883</v>
@@ -3315,7 +3420,7 @@
         <v>0.0151856886949631</v>
       </c>
       <c r="E35">
-        <v>0.0513519462672571</v>
+        <v>0.051802542937245</v>
       </c>
       <c r="F35">
         <v>5.68157241573899e-05</v>
@@ -3366,24 +3471,27 @@
         <v>2.94392706621614</v>
       </c>
       <c r="V35">
-        <v>0.931232742432657</v>
+        <v>0.931232742432658</v>
       </c>
       <c r="W35">
         <v>-0.824144253910764</v>
       </c>
       <c r="X35">
-        <v>-0.476886507417701</v>
+        <v>-1.27954169710482</v>
       </c>
       <c r="Y35">
         <v>0.0139078463835676</v>
       </c>
       <c r="Z35">
-        <v>-0.423461310587128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26">
+        <v>-0.641753705396268</v>
+      </c>
+      <c r="AA35">
+        <v>0.968744140452917</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B36">
         <v>0.0129300524037366</v>
@@ -3395,7 +3503,7 @@
         <v>0.021406743785209</v>
       </c>
       <c r="E36">
-        <v>0.0516106236237534</v>
+        <v>0.0515844976432836</v>
       </c>
       <c r="F36">
         <v>0.0215311173590645</v>
@@ -3410,7 +3518,7 @@
         <v>0.475553674381394</v>
       </c>
       <c r="J36">
-        <v>0.0618976942766489</v>
+        <v>0.0618976942766539</v>
       </c>
       <c r="K36">
         <v>-0.272013123310375</v>
@@ -3452,18 +3560,21 @@
         <v>1.51776277387999</v>
       </c>
       <c r="X36">
-        <v>-0.502199110377616</v>
+        <v>-0.509813291662868</v>
       </c>
       <c r="Y36">
         <v>0.0159379240949826</v>
       </c>
       <c r="Z36">
-        <v>0.480411548468463</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26">
+        <v>0.616290782663778</v>
+      </c>
+      <c r="AA36">
+        <v>1.10770841969219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B37">
         <v>0.019378683448207</v>
@@ -3475,7 +3586,7 @@
         <v>0.0127431254191818</v>
       </c>
       <c r="E37">
-        <v>0.0583419618778432</v>
+        <v>0.0585702453224278</v>
       </c>
       <c r="F37">
         <v>0.00394883301773006</v>
@@ -3532,18 +3643,21 @@
         <v>0.709658773503338</v>
       </c>
       <c r="X37">
-        <v>-1.10056725999374</v>
+        <v>-1.61438638904221</v>
       </c>
       <c r="Y37">
         <v>0.0145325579534586</v>
       </c>
       <c r="Z37">
-        <v>-0.783987280782335</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26">
+        <v>-0.80704493633994</v>
+      </c>
+      <c r="AA37">
+        <v>0.847050069997274</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B38">
         <v>0.0166122004357298</v>
@@ -3612,18 +3726,21 @@
         <v>-2.07262794079266</v>
       </c>
       <c r="X38">
-        <v>-2.43173415364865</v>
+        <v>-0.629600912658276</v>
       </c>
       <c r="Y38">
         <v>0.0165550813212645</v>
       </c>
       <c r="Z38">
-        <v>0.422904832153044</v>
-      </c>
-    </row>
-    <row r="39" spans="1:26">
+        <v>0.703545832112202</v>
+      </c>
+      <c r="AA38">
+        <v>1.0703991782136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B39">
         <v>0.0117889773062187</v>
@@ -3650,7 +3767,7 @@
         <v>0.404298244043134</v>
       </c>
       <c r="J39">
-        <v>0.0768814325141876</v>
+        <v>0.0768814325141798</v>
       </c>
       <c r="K39">
         <v>-0.26293492117317</v>
@@ -3692,18 +3809,21 @@
         <v>-0.400862997033865</v>
       </c>
       <c r="X39">
-        <v>-0.641763364787853</v>
+        <v>-1.97398078997437</v>
       </c>
       <c r="Y39">
         <v>0.0174159070567434</v>
       </c>
       <c r="Z39">
-        <v>0.452081820990334</v>
-      </c>
-    </row>
-    <row r="40" spans="1:26">
+        <v>-0.136136271283011</v>
+      </c>
+      <c r="AA39">
+        <v>1.06547540132603</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B40">
         <v>0.018018018018018</v>
@@ -3715,7 +3835,7 @@
         <v>0.0226640318604604</v>
       </c>
       <c r="E40">
-        <v>0.055595312623296</v>
+        <v>0.0555953126232959</v>
       </c>
       <c r="F40">
         <v>0.0423586679624272</v>
@@ -3766,24 +3886,27 @@
         <v>4.46947547692328</v>
       </c>
       <c r="V40">
-        <v>0.909879266755755</v>
+        <v>0.909879266755756</v>
       </c>
       <c r="W40">
         <v>1.2102469506713</v>
       </c>
       <c r="X40">
-        <v>0.353229549039373</v>
+        <v>0.043896318012567</v>
       </c>
       <c r="Y40">
         <v>0.0146197522283737</v>
       </c>
       <c r="Z40">
-        <v>0.471688320769116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:26">
+        <v>0.510529242897941</v>
+      </c>
+      <c r="AA40">
+        <v>0.939497303142611</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B41">
         <v>0.0218181818181818</v>
@@ -3795,7 +3918,7 @@
         <v>0.022487502466666</v>
       </c>
       <c r="E41">
-        <v>0.065151331707877</v>
+        <v>0.065612318978133</v>
       </c>
       <c r="F41">
         <v>0.0465857645278992</v>
@@ -3810,7 +3933,7 @@
         <v>0.37828465028424</v>
       </c>
       <c r="J41">
-        <v>0.0486754109713452</v>
+        <v>0.0486754109713461</v>
       </c>
       <c r="K41">
         <v>-0.253422772445006</v>
@@ -3852,18 +3975,21 @@
         <v>-0.787205708643641</v>
       </c>
       <c r="X41">
-        <v>-1.19562962751351</v>
+        <v>-0.768297283738676</v>
       </c>
       <c r="Y41">
         <v>0.0157797226669743</v>
       </c>
       <c r="Z41">
-        <v>-0.469603947214267</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26">
+        <v>-0.379190299319217</v>
+      </c>
+      <c r="AA41">
+        <v>1.02138039698852</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B42">
         <v>0.0493951612903226</v>
@@ -3932,18 +4058,21 @@
         <v>-0.449599716257388</v>
       </c>
       <c r="X42">
-        <v>-0.463277133439548</v>
+        <v>-0.752437583271655</v>
       </c>
       <c r="Y42">
         <v>0.00944419553063511</v>
       </c>
       <c r="Z42">
-        <v>0.315437049228035</v>
-      </c>
-    </row>
-    <row r="43" spans="1:26">
+        <v>0.209652451905611</v>
+      </c>
+      <c r="AA42">
+        <v>0.67358089270154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B43">
         <v>0.2</v>
@@ -4012,18 +4141,21 @@
         <v>-1.72972907025383</v>
       </c>
       <c r="X43">
-        <v>-0.588206213144471</v>
+        <v>-1.42126647326338</v>
       </c>
       <c r="Y43">
         <v>0.00642756742316938</v>
       </c>
       <c r="Z43">
-        <v>-0.665712460449281</v>
-      </c>
-    </row>
-    <row r="44" spans="1:26">
+        <v>-0.764439938540495</v>
+      </c>
+      <c r="AA43">
+        <v>0.316045913814248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B44">
         <v>0.106617647058824</v>
@@ -4035,7 +4167,7 @@
         <v>0.0941176470588235</v>
       </c>
       <c r="E44">
-        <v>0.180673724972677</v>
+        <v>0.17223487960862</v>
       </c>
       <c r="F44">
         <v>0.212197700127084</v>
@@ -4092,18 +4224,21 @@
         <v>0.292188771086001</v>
       </c>
       <c r="X44">
-        <v>1.14788863800419</v>
+        <v>1.1873924357676</v>
       </c>
       <c r="Y44">
         <v>0.00861579736784824</v>
       </c>
       <c r="Z44">
-        <v>0.764681305765744</v>
-      </c>
-    </row>
-    <row r="45" spans="1:26">
+        <v>0.849594794451561</v>
+      </c>
+      <c r="AA44">
+        <v>1.88897245302525</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27">
       <c r="A45" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B45">
         <v>0.357142857142857</v>
@@ -4172,13 +4307,16 @@
         <v>0.303596422697832</v>
       </c>
       <c r="X45">
-        <v>-0.466096463939456</v>
+        <v>-0.328380254229133</v>
       </c>
       <c r="Y45">
         <v>0.0133162403328807</v>
       </c>
       <c r="Z45">
-        <v>-0.106927494084415</v>
+        <v>-0.210662437797451</v>
+      </c>
+      <c r="AA45">
+        <v>0.692824659123163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "stationarity calculations, fk and radon plots"
This reverts commit 625f2ab2cbe526fdfbfead84f626de2bee2f0720.

# Conflicts:
#	Thesis/Code/.ipynb_checkpoints/Dynamic Network Analysis
00-checkpoint.ipynb
#	Thesis/Code/Dynamic Network Analysis 00.ipynb
</commit_message>
<xml_diff>
--- a/Thesis/Code/enron_dynet_attvol.xlsx
+++ b/Thesis/Code/enron_dynet_attvol.xlsx
@@ -85,13 +85,13 @@
     <t>LogICARatio</t>
   </si>
   <si>
+    <t>NormNMFRatio</t>
+  </si>
+  <si>
     <t>SubgraphStat</t>
   </si>
   <si>
     <t>Emergence</t>
-  </si>
-  <si>
-    <t>NormNMFRatio</t>
   </si>
   <si>
     <t>Nov98</t>
@@ -779,7 +779,7 @@
         <v>0.246464646464646</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0.999999999999998</v>
       </c>
       <c r="K3">
         <v>-0.199212484783527</v>
@@ -821,16 +821,16 @@
         <v>-0.310794340746057</v>
       </c>
       <c r="X3">
-        <v>0.355047508500758</v>
+        <v>1.04887005367672</v>
       </c>
       <c r="Y3">
+        <v>1.47806084097062</v>
+      </c>
+      <c r="Z3">
         <v>0.0130686392313725</v>
       </c>
-      <c r="Z3">
-        <v>0.485409215907839</v>
-      </c>
       <c r="AA3">
-        <v>1.47806084097062</v>
+        <v>0.497251009589878</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -904,16 +904,16 @@
         <v>0.538397982609507</v>
       </c>
       <c r="X4">
-        <v>1.43726655438487</v>
+        <v>1.34588594833288</v>
       </c>
       <c r="Y4">
+        <v>0.89568857487168</v>
+      </c>
+      <c r="Z4">
         <v>0.0157442604741007</v>
       </c>
-      <c r="Z4">
-        <v>0.0187120544090581</v>
-      </c>
       <c r="AA4">
-        <v>0.89568857487168</v>
+        <v>-0.0179800374934191</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -987,16 +987,16 @@
         <v>-1.05191082665109</v>
       </c>
       <c r="X5">
-        <v>-0.682907060830884</v>
+        <v>-0.853645217176353</v>
       </c>
       <c r="Y5">
+        <v>0.487905759876115</v>
+      </c>
+      <c r="Z5">
         <v>0.00878987146533087</v>
       </c>
-      <c r="Z5">
-        <v>-0.155184651760784</v>
-      </c>
       <c r="AA5">
-        <v>0.487905759876115</v>
+        <v>-0.144898012301384</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -1028,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.999999999999999</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>-0.157405383455039</v>
@@ -1070,16 +1070,16 @@
         <v>1.69741990976954</v>
       </c>
       <c r="X6">
-        <v>0.986995014038095</v>
+        <v>0.614796557862919</v>
       </c>
       <c r="Y6">
+        <v>1.31832895468212</v>
+      </c>
+      <c r="Z6">
         <v>0.0124307554377872</v>
       </c>
-      <c r="Z6">
-        <v>0.297927735126215</v>
-      </c>
       <c r="AA6">
-        <v>1.31832895468212</v>
+        <v>0.263660888901169</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1153,16 +1153,16 @@
         <v>-1.69741990976954</v>
       </c>
       <c r="X7">
-        <v>-1.19139090968465</v>
+        <v>0.270097535571253</v>
       </c>
       <c r="Y7">
+        <v>0.75853602126271</v>
+      </c>
+      <c r="Z7">
         <v>0.0124307554377872</v>
       </c>
-      <c r="Z7">
-        <v>-0.378621196499424</v>
-      </c>
       <c r="AA7">
-        <v>0.75853602126271</v>
+        <v>-0.206038554769815</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -1236,16 +1236,16 @@
         <v>1.04529271084357</v>
       </c>
       <c r="X8">
-        <v>0.429239578071182</v>
+        <v>1.22434314905709</v>
       </c>
       <c r="Y8">
+        <v>2.01279597217926</v>
+      </c>
+      <c r="Z8">
         <v>0.0070118917343666</v>
       </c>
-      <c r="Z8">
-        <v>0.302081121206406</v>
-      </c>
       <c r="AA8">
-        <v>2.01279597217926</v>
+        <v>0.186687152903642</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1319,16 +1319,16 @@
         <v>14.0709202030539</v>
       </c>
       <c r="X9">
-        <v>1.05723215840821</v>
+        <v>1.78523177094415</v>
       </c>
       <c r="Y9">
+        <v>0.908884467951915</v>
+      </c>
+      <c r="Z9">
         <v>0.0145159949751711</v>
       </c>
-      <c r="Z9">
-        <v>0.48966865698235</v>
-      </c>
       <c r="AA9">
-        <v>0.908884467951915</v>
+        <v>0.47136943766907</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1360,7 +1360,7 @@
         <v>0.387962962962963</v>
       </c>
       <c r="J10">
-        <v>0.238465591590027</v>
+        <v>0.238465591590029</v>
       </c>
       <c r="K10">
         <v>-0.176051138447516</v>
@@ -1402,16 +1402,16 @@
         <v>-13.6340352261333</v>
       </c>
       <c r="X10">
-        <v>-1.10049676408314</v>
+        <v>-1.00281087588735</v>
       </c>
       <c r="Y10">
+        <v>1.72134344587126</v>
+      </c>
+      <c r="Z10">
         <v>0.0131379693689775</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>-1</v>
-      </c>
-      <c r="AA10">
-        <v>1.72134344587126</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -1485,16 +1485,16 @@
         <v>-0.192578685742613</v>
       </c>
       <c r="X11">
-        <v>0.333995250421391</v>
+        <v>0.766294317803198</v>
       </c>
       <c r="Y11">
+        <v>0.817432300754284</v>
+      </c>
+      <c r="Z11">
         <v>0.0150361523392413</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>1</v>
-      </c>
-      <c r="AA11">
-        <v>0.817432300754284</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -1568,16 +1568,16 @@
         <v>1.0337269710037</v>
       </c>
       <c r="X12">
-        <v>-1.01153684225008</v>
+        <v>0.576757883719376</v>
       </c>
       <c r="Y12">
+        <v>1.22070400001624</v>
+      </c>
+      <c r="Z12">
         <v>0.0140866989190509</v>
       </c>
-      <c r="Z12">
-        <v>0.00625326125694494</v>
-      </c>
       <c r="AA12">
-        <v>1.22070400001624</v>
+        <v>0.207610035607276</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -1651,16 +1651,16 @@
         <v>-1.63461113465214</v>
       </c>
       <c r="X13">
-        <v>-0.804111484444151</v>
+        <v>-1.18834813707523</v>
       </c>
       <c r="Y13">
+        <v>1.26845788294828</v>
+      </c>
+      <c r="Z13">
         <v>0.0154534567266276</v>
       </c>
-      <c r="Z13">
-        <v>-0.429681316969979</v>
-      </c>
       <c r="AA13">
-        <v>1.26845788294828</v>
+        <v>-0.504563175973437</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -1734,16 +1734,16 @@
         <v>2.22407908330382</v>
       </c>
       <c r="X14">
-        <v>-1.2835483451852</v>
+        <v>-0.306078378431768</v>
       </c>
       <c r="Y14">
+        <v>0.603924264107491</v>
+      </c>
+      <c r="Z14">
         <v>0.0160828854606541</v>
       </c>
-      <c r="Z14">
-        <v>0.499565787028071</v>
-      </c>
       <c r="AA14">
-        <v>0.603924264107491</v>
+        <v>0.508278477296733</v>
       </c>
     </row>
     <row r="15" spans="1:27">
@@ -1817,16 +1817,16 @@
         <v>0.700871081985116</v>
       </c>
       <c r="X15">
-        <v>1.40446799016771</v>
+        <v>1.38816303780057</v>
       </c>
       <c r="Y15">
+        <v>3.47512635591994</v>
+      </c>
+      <c r="Z15">
         <v>0.0113929755478287</v>
       </c>
-      <c r="Z15">
-        <v>0.0440367493189775</v>
-      </c>
       <c r="AA15">
-        <v>3.47512635591994</v>
+        <v>0.0202201338050722</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -1900,16 +1900,16 @@
         <v>-2.8331062521871</v>
       </c>
       <c r="X16">
-        <v>-0.204270994099142</v>
+        <v>-0.979063228217563</v>
       </c>
       <c r="Y16">
+        <v>0.648501521447253</v>
+      </c>
+      <c r="Z16">
         <v>0.0145604426441847</v>
       </c>
-      <c r="Z16">
-        <v>-0.708034937602533</v>
-      </c>
       <c r="AA16">
-        <v>0.648501521447253</v>
+        <v>-0.71971545076833</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -1983,16 +1983,16 @@
         <v>1.17264436501075</v>
       </c>
       <c r="X17">
-        <v>-0.277466947794664</v>
+        <v>-0.285897814894531</v>
       </c>
       <c r="Y17">
+        <v>0.986712034676278</v>
+      </c>
+      <c r="Z17">
         <v>0.014825334134991</v>
       </c>
-      <c r="Z17">
-        <v>0.672292340219475</v>
-      </c>
       <c r="AA17">
-        <v>0.986712034676278</v>
+        <v>0.655269943305426</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -2024,7 +2024,7 @@
         <v>0.235756360756361</v>
       </c>
       <c r="J18">
-        <v>0.0646489545249898</v>
+        <v>0.0646489545249885</v>
       </c>
       <c r="K18">
         <v>-0.237276142988631</v>
@@ -2066,16 +2066,16 @@
         <v>-0.246935913586076</v>
       </c>
       <c r="X18">
-        <v>0.134541549332513</v>
+        <v>-1.08268963872178</v>
       </c>
       <c r="Y18">
+        <v>1.15017241711094</v>
+      </c>
+      <c r="Z18">
         <v>0.0153540765528727</v>
       </c>
-      <c r="Z18">
-        <v>-0.201712149724085</v>
-      </c>
       <c r="AA18">
-        <v>1.15017241711094</v>
+        <v>-0.248977703341267</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -2149,16 +2149,16 @@
         <v>-0.370739975058558</v>
       </c>
       <c r="X19">
-        <v>-1.3451979492215</v>
+        <v>2.41117600821318</v>
       </c>
       <c r="Y19">
+        <v>1.06896439663969</v>
+      </c>
+      <c r="Z19">
         <v>0.0158764726629214</v>
       </c>
-      <c r="Z19">
-        <v>0.277950671015695</v>
-      </c>
       <c r="AA19">
-        <v>1.06896439663969</v>
+        <v>0.524839242191961</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -2232,16 +2232,16 @@
         <v>1.05075613713745</v>
       </c>
       <c r="X20">
-        <v>3.61505799642203</v>
+        <v>1.40976557261538</v>
       </c>
       <c r="Y20">
+        <v>0.907380390841924</v>
+      </c>
+      <c r="Z20">
         <v>0.0141937749294579</v>
       </c>
-      <c r="Z20">
-        <v>0.0472228955487312</v>
-      </c>
       <c r="AA20">
-        <v>0.907380390841924</v>
+        <v>-0.367113848097586</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -2315,16 +2315,16 @@
         <v>1.145740474131</v>
       </c>
       <c r="X21">
-        <v>-0.323226998341732</v>
+        <v>0.562431634653335</v>
       </c>
       <c r="Y21">
+        <v>0.993876622141327</v>
+      </c>
+      <c r="Z21">
         <v>0.0145117123390032</v>
       </c>
-      <c r="Z21">
-        <v>-0.265848917549648</v>
-      </c>
       <c r="AA21">
-        <v>0.993876622141327</v>
+        <v>0.0495124643559382</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -2398,16 +2398,16 @@
         <v>-1.50978661909184</v>
       </c>
       <c r="X22">
-        <v>-0.224611224193025</v>
+        <v>0.439728819521156</v>
       </c>
       <c r="Y22">
+        <v>1.14969210902986</v>
+      </c>
+      <c r="Z22">
         <v>0.014594047644061</v>
       </c>
-      <c r="Z22">
-        <v>-0.0177951937566633</v>
-      </c>
       <c r="AA22">
-        <v>1.14969210902986</v>
+        <v>-0.0658626360806904</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -2481,16 +2481,16 @@
         <v>1.12579431337031</v>
       </c>
       <c r="X23">
-        <v>0.566559629994456</v>
+        <v>-1.41525850893781</v>
       </c>
       <c r="Y23">
+        <v>0.823466610119958</v>
+      </c>
+      <c r="Z23">
         <v>0.014389861392556</v>
       </c>
-      <c r="Z23">
-        <v>-0.190533185638212</v>
-      </c>
       <c r="AA23">
-        <v>0.823466610119958</v>
+        <v>-0.459535599239836</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -2564,16 +2564,16 @@
         <v>-0.541538212690746</v>
       </c>
       <c r="X24">
-        <v>0.445841546612435</v>
+        <v>-2.70338416780498</v>
       </c>
       <c r="Y24">
+        <v>6.36640412963768</v>
+      </c>
+      <c r="Z24">
         <v>0.0161524545736765</v>
       </c>
-      <c r="Z24">
-        <v>0.452650931285279</v>
-      </c>
       <c r="AA24">
-        <v>6.36640412963768</v>
+        <v>0.455185284677532</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -2647,16 +2647,16 @@
         <v>-0.40115131886765</v>
       </c>
       <c r="X25">
-        <v>-0.0141925663441352</v>
+        <v>0.354501699724576</v>
       </c>
       <c r="Y25">
+        <v>0.158850872775147</v>
+      </c>
+      <c r="Z25">
         <v>0.0153914881537371</v>
       </c>
-      <c r="Z25">
-        <v>-0.568600024615127</v>
-      </c>
       <c r="AA25">
-        <v>0.158850872775147</v>
+        <v>-0.3333077950483</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -2730,16 +2730,16 @@
         <v>0.0650015997574016</v>
       </c>
       <c r="X26">
-        <v>-0.301618269630589</v>
+        <v>-1.49678311568755</v>
       </c>
       <c r="Y26">
+        <v>2.31070909967728</v>
+      </c>
+      <c r="Z26">
         <v>0.0157083458970645</v>
       </c>
-      <c r="Z26">
-        <v>0.290270924639705</v>
-      </c>
       <c r="AA26">
-        <v>2.31070909967728</v>
+        <v>0.0221415726462084</v>
       </c>
     </row>
     <row r="27" spans="1:27">
@@ -2813,16 +2813,16 @@
         <v>-0.141684921779725</v>
       </c>
       <c r="X27">
-        <v>1.70875345594072</v>
+        <v>1.38151543494553</v>
       </c>
       <c r="Y27">
+        <v>0.487947303386618</v>
+      </c>
+      <c r="Z27">
         <v>0.0154573970921823</v>
       </c>
-      <c r="Z27">
-        <v>0.181863517060296</v>
-      </c>
       <c r="AA27">
-        <v>0.487947303386618</v>
+        <v>0.273807624878081</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -2896,16 +2896,16 @@
         <v>-0.491368424547045</v>
       </c>
       <c r="X28">
-        <v>0.739502362394502</v>
+        <v>0.154986937700053</v>
       </c>
       <c r="Y28">
+        <v>0.938555672609553</v>
+      </c>
+      <c r="Z28">
         <v>0.0159509673976893</v>
       </c>
-      <c r="Z28">
-        <v>-0.362684784623684</v>
-      </c>
       <c r="AA28">
-        <v>0.938555672609553</v>
+        <v>-0.329200170677304</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -2979,16 +2979,16 @@
         <v>-0.225297129925138</v>
       </c>
       <c r="X29">
-        <v>0.599420682217894</v>
+        <v>-0.934557070631527</v>
       </c>
       <c r="Y29">
+        <v>1.19335042512633</v>
+      </c>
+      <c r="Z29">
         <v>0.0163705868910213</v>
       </c>
-      <c r="Z29">
-        <v>-0.0319605398737786</v>
-      </c>
       <c r="AA29">
-        <v>1.19335042512633</v>
+        <v>-0.264164328800264</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -3062,16 +3062,16 @@
         <v>0.227354792574308</v>
       </c>
       <c r="X30">
-        <v>0.0888315252844555</v>
+        <v>0.139227600919719</v>
       </c>
       <c r="Y30">
+        <v>0.946094252235949</v>
+      </c>
+      <c r="Z30">
         <v>0.0156018477241692</v>
       </c>
-      <c r="Z30">
-        <v>0.156708865525271</v>
-      </c>
       <c r="AA30">
-        <v>0.946094252235949</v>
+        <v>0.362055877466574</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -3145,16 +3145,16 @@
         <v>1.30380508791649</v>
       </c>
       <c r="X31">
-        <v>-2.21678463990497</v>
+        <v>-0.828633894425627</v>
       </c>
       <c r="Y31">
+        <v>0.904090206526913</v>
+      </c>
+      <c r="Z31">
         <v>0.0155941129759143</v>
       </c>
-      <c r="Z31">
-        <v>-0.367164455694182</v>
-      </c>
       <c r="AA31">
-        <v>0.904090206526913</v>
+        <v>-0.067430633608431</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -3228,16 +3228,16 @@
         <v>-0.485540704138178</v>
       </c>
       <c r="X32">
-        <v>-0.893012985764048</v>
+        <v>-2.5875680790163</v>
       </c>
       <c r="Y32">
+        <v>1.05616235065536</v>
+      </c>
+      <c r="Z32">
         <v>0.0155906223665728</v>
       </c>
-      <c r="Z32">
-        <v>-0.0246133482319035</v>
-      </c>
       <c r="AA32">
-        <v>1.05616235065536</v>
+        <v>-0.590480977984785</v>
       </c>
     </row>
     <row r="33" spans="1:27">
@@ -3311,16 +3311,16 @@
         <v>-0.730432509767316</v>
       </c>
       <c r="X33">
-        <v>-0.571122678617127</v>
+        <v>0.913687368325867</v>
       </c>
       <c r="Y33">
+        <v>0.989825199424454</v>
+      </c>
+      <c r="Z33">
         <v>0.0164239032884816</v>
       </c>
-      <c r="Z33">
-        <v>0.572047289486678</v>
-      </c>
       <c r="AA33">
-        <v>0.989825199424454</v>
+        <v>0.763038460876312</v>
       </c>
     </row>
     <row r="34" spans="1:27">
@@ -3394,16 +3394,16 @@
         <v>1.41127049960005</v>
       </c>
       <c r="X34">
-        <v>1.0709850128508</v>
+        <v>1.09501346185881</v>
       </c>
       <c r="Y34">
+        <v>0.963061159874462</v>
+      </c>
+      <c r="Z34">
         <v>0.0144777445925457</v>
       </c>
-      <c r="Z34">
-        <v>0.0382293318183974</v>
-      </c>
       <c r="AA34">
-        <v>0.963061159874462</v>
+        <v>-0.0483531435235984</v>
       </c>
     </row>
     <row r="35" spans="1:27">
@@ -3477,16 +3477,16 @@
         <v>-0.824144253910764</v>
       </c>
       <c r="X35">
-        <v>-1.27954169710482</v>
+        <v>0.121835458367477</v>
       </c>
       <c r="Y35">
+        <v>0.968744140452917</v>
+      </c>
+      <c r="Z35">
         <v>0.0139078463835676</v>
       </c>
-      <c r="Z35">
-        <v>-0.641753705396268</v>
-      </c>
       <c r="AA35">
-        <v>0.968744140452917</v>
+        <v>-0.423828515486821</v>
       </c>
     </row>
     <row r="36" spans="1:27">
@@ -3518,7 +3518,7 @@
         <v>0.475553674381394</v>
       </c>
       <c r="J36">
-        <v>0.0618976942766539</v>
+        <v>0.0618976942766494</v>
       </c>
       <c r="K36">
         <v>-0.272013123310375</v>
@@ -3560,16 +3560,16 @@
         <v>1.51776277387999</v>
       </c>
       <c r="X36">
-        <v>-0.509813291662868</v>
+        <v>-1.15232183184174</v>
       </c>
       <c r="Y36">
+        <v>1.10770841969219</v>
+      </c>
+      <c r="Z36">
         <v>0.0159379240949826</v>
       </c>
-      <c r="Z36">
-        <v>0.616290782663778</v>
-      </c>
       <c r="AA36">
-        <v>1.10770841969219</v>
+        <v>0.281001650138757</v>
       </c>
     </row>
     <row r="37" spans="1:27">
@@ -3643,16 +3643,16 @@
         <v>0.709658773503338</v>
       </c>
       <c r="X37">
-        <v>-1.61438638904221</v>
+        <v>-0.801510330820907</v>
       </c>
       <c r="Y37">
+        <v>0.847050069997274</v>
+      </c>
+      <c r="Z37">
         <v>0.0145325579534586</v>
       </c>
-      <c r="Z37">
-        <v>-0.80704493633994</v>
-      </c>
       <c r="AA37">
-        <v>0.847050069997274</v>
+        <v>-0.557419284141504</v>
       </c>
     </row>
     <row r="38" spans="1:27">
@@ -3726,16 +3726,16 @@
         <v>-2.07262794079266</v>
       </c>
       <c r="X38">
-        <v>-0.629600912658276</v>
+        <v>0.566837583827508</v>
       </c>
       <c r="Y38">
+        <v>1.0703991782136</v>
+      </c>
+      <c r="Z38">
         <v>0.0165550813212645</v>
       </c>
-      <c r="Z38">
-        <v>0.703545832112202</v>
-      </c>
       <c r="AA38">
-        <v>1.0703991782136</v>
+        <v>0.455274433787522</v>
       </c>
     </row>
     <row r="39" spans="1:27">
@@ -3767,7 +3767,7 @@
         <v>0.404298244043134</v>
       </c>
       <c r="J39">
-        <v>0.0768814325141798</v>
+        <v>0.0768814325141799</v>
       </c>
       <c r="K39">
         <v>-0.26293492117317</v>
@@ -3809,16 +3809,16 @@
         <v>-0.400862997033865</v>
       </c>
       <c r="X39">
-        <v>-1.97398078997437</v>
+        <v>0.48768383003101</v>
       </c>
       <c r="Y39">
+        <v>1.06547540132603</v>
+      </c>
+      <c r="Z39">
         <v>0.0174159070567434</v>
       </c>
-      <c r="Z39">
-        <v>-0.136136271283011</v>
-      </c>
       <c r="AA39">
-        <v>1.06547540132603</v>
+        <v>0.175574785184368</v>
       </c>
     </row>
     <row r="40" spans="1:27">
@@ -3886,22 +3886,22 @@
         <v>4.46947547692328</v>
       </c>
       <c r="V40">
-        <v>0.909879266755756</v>
+        <v>0.909879266755755</v>
       </c>
       <c r="W40">
         <v>1.2102469506713</v>
       </c>
       <c r="X40">
-        <v>0.043896318012567</v>
+        <v>-0.587404322954513</v>
       </c>
       <c r="Y40">
+        <v>0.939497303142611</v>
+      </c>
+      <c r="Z40">
         <v>0.0146197522283737</v>
       </c>
-      <c r="Z40">
-        <v>0.510529242897941</v>
-      </c>
       <c r="AA40">
-        <v>0.939497303142611</v>
+        <v>0.172025904277018</v>
       </c>
     </row>
     <row r="41" spans="1:27">
@@ -3933,7 +3933,7 @@
         <v>0.37828465028424</v>
       </c>
       <c r="J41">
-        <v>0.0486754109713461</v>
+        <v>0.048675410971366</v>
       </c>
       <c r="K41">
         <v>-0.253422772445006</v>
@@ -3975,16 +3975,16 @@
         <v>-0.787205708643641</v>
       </c>
       <c r="X41">
-        <v>-0.768297283738676</v>
+        <v>-1.69455934132459</v>
       </c>
       <c r="Y41">
+        <v>1.02138039698852</v>
+      </c>
+      <c r="Z41">
         <v>0.0157797226669743</v>
       </c>
-      <c r="Z41">
-        <v>-0.379190299319217</v>
-      </c>
       <c r="AA41">
-        <v>1.02138039698852</v>
+        <v>-0.354922469674246</v>
       </c>
     </row>
     <row r="42" spans="1:27">
@@ -4058,16 +4058,16 @@
         <v>-0.449599716257388</v>
       </c>
       <c r="X42">
-        <v>-0.752437583271655</v>
+        <v>-0.480404067142626</v>
       </c>
       <c r="Y42">
+        <v>0.67358089270154</v>
+      </c>
+      <c r="Z42">
         <v>0.00944419553063511</v>
       </c>
-      <c r="Z42">
-        <v>0.209652451905611</v>
-      </c>
       <c r="AA42">
-        <v>0.67358089270154</v>
+        <v>0.2746462865345</v>
       </c>
     </row>
     <row r="43" spans="1:27">
@@ -4141,16 +4141,16 @@
         <v>-1.72972907025383</v>
       </c>
       <c r="X43">
-        <v>-1.42126647326338</v>
+        <v>-2.20627013906616</v>
       </c>
       <c r="Y43">
+        <v>0.316045913814248</v>
+      </c>
+      <c r="Z43">
         <v>0.00642756742316938</v>
       </c>
-      <c r="Z43">
-        <v>-0.764439938540495</v>
-      </c>
       <c r="AA43">
-        <v>0.316045913814248</v>
+        <v>-0.760420169006862</v>
       </c>
     </row>
     <row r="44" spans="1:27">
@@ -4182,7 +4182,7 @@
         <v>0.198039215686274</v>
       </c>
       <c r="J44">
-        <v>0.181213264532619</v>
+        <v>0.18121326453262</v>
       </c>
       <c r="K44">
         <v>-0.187750022430375</v>
@@ -4224,16 +4224,16 @@
         <v>0.292188771086001</v>
       </c>
       <c r="X44">
-        <v>1.1873924357676</v>
+        <v>1.25358684555304</v>
       </c>
       <c r="Y44">
+        <v>1.88897245302525</v>
+      </c>
+      <c r="Z44">
         <v>0.00861579736784824</v>
       </c>
-      <c r="Z44">
-        <v>0.849594794451561</v>
-      </c>
       <c r="AA44">
-        <v>1.88897245302525</v>
+        <v>0.836037129462003</v>
       </c>
     </row>
     <row r="45" spans="1:27">
@@ -4307,16 +4307,16 @@
         <v>0.303596422697832</v>
       </c>
       <c r="X45">
-        <v>-0.328380254229133</v>
+        <v>-0.854212213859845</v>
       </c>
       <c r="Y45">
+        <v>0.692824659123163</v>
+      </c>
+      <c r="Z45">
         <v>0.0133162403328807</v>
       </c>
-      <c r="Z45">
-        <v>-0.210662437797451</v>
-      </c>
       <c r="AA45">
-        <v>0.692824659123163</v>
+        <v>-0.187871788619365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated folder structure and sofication analysis
</commit_message>
<xml_diff>
--- a/Thesis/Code/enron_dynet_attvol.xlsx
+++ b/Thesis/Code/enron_dynet_attvol.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>AvgDeg</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>IAwIP</t>
+  </si>
+  <si>
+    <t>Power</t>
   </si>
   <si>
     <t>MeanResistanceDist</t>
@@ -581,13 +584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA45"/>
+  <dimension ref="A1:AB45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:28">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,10 +669,13 @@
       <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:28">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0.142857142857143</v>
@@ -681,7 +687,7 @@
         <v>0.125</v>
       </c>
       <c r="E2">
-        <v>0.222018968604531</v>
+        <v>1.45716771982052e-16</v>
       </c>
       <c r="F2">
         <v>0.18543463409279</v>
@@ -729,13 +735,13 @@
         <v>0.345301423907833</v>
       </c>
       <c r="U2">
+        <v>0.76730190262563</v>
+      </c>
+      <c r="V2">
         <v>1.60383986423538</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>0.894427190999916</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
       </c>
       <c r="X2">
         <v>0</v>
@@ -749,10 +755,13 @@
       <c r="AA2">
         <v>0</v>
       </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:28">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>0.145454545454545</v>
@@ -764,10 +773,10 @@
         <v>0.0868686868686869</v>
       </c>
       <c r="E3">
-        <v>0.233759914226578</v>
+        <v>0.198999299503384</v>
       </c>
       <c r="F3">
-        <v>0.175110542980077</v>
+        <v>0.198999326241596</v>
       </c>
       <c r="G3">
         <v>0.0868686868686869</v>
@@ -779,7 +788,7 @@
         <v>0.246464646464646</v>
       </c>
       <c r="J3">
-        <v>0.999999999999998</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>-0.199212484783527</v>
@@ -794,7 +803,7 @@
         <v>0.241116635589403</v>
       </c>
       <c r="O3">
-        <v>0.00872589419574727</v>
+        <v>0.00872589419574728</v>
       </c>
       <c r="P3">
         <v>-0.00942284041170726</v>
@@ -812,30 +821,33 @@
         <v>1.25514048155862</v>
       </c>
       <c r="U3">
+        <v>0.597478474794714</v>
+      </c>
+      <c r="V3">
         <v>1.80404959028772</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>0.908295106229248</v>
       </c>
-      <c r="W3">
-        <v>-0.310794340746057</v>
-      </c>
       <c r="X3">
-        <v>1.04887005367672</v>
+        <v>-0.614383454515078</v>
       </c>
       <c r="Y3">
-        <v>1.47806084097062</v>
+        <v>0.502137074301377</v>
       </c>
       <c r="Z3">
+        <v>1.65520906507215</v>
+      </c>
+      <c r="AA3">
         <v>0.0130686392313725</v>
       </c>
-      <c r="AA3">
-        <v>0.497251009589878</v>
+      <c r="AB3">
+        <v>0.445441605104984</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:28">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>0.0833333333333333</v>
@@ -847,7 +859,7 @@
         <v>0.0769230769230769</v>
       </c>
       <c r="E4">
-        <v>0.132902115949708</v>
+        <v>3.20256641718795e-17</v>
       </c>
       <c r="F4">
         <v>0.0576923076923077</v>
@@ -895,30 +907,33 @@
         <v>2.26563421242698</v>
       </c>
       <c r="U4">
+        <v>0.502681401566927</v>
+      </c>
+      <c r="V4">
         <v>1.75126687346235</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>0.930949336251263</v>
       </c>
-      <c r="W4">
-        <v>0.538397982609507</v>
-      </c>
       <c r="X4">
-        <v>1.34588594833288</v>
+        <v>0.387559752143189</v>
       </c>
       <c r="Y4">
-        <v>0.89568857487168</v>
+        <v>0.407074691226119</v>
       </c>
       <c r="Z4">
+        <v>0.850969427275761</v>
+      </c>
+      <c r="AA4">
         <v>0.0157442604741007</v>
       </c>
-      <c r="AA4">
-        <v>-0.0179800374934191</v>
+      <c r="AB4">
+        <v>-0.0777767301315639</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:28">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -978,30 +993,33 @@
         <v>2.71409499247695</v>
       </c>
       <c r="U5">
+        <v>2.10987192594582</v>
+      </c>
+      <c r="V5">
         <v>0.99046817359701</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>0.774596669241483</v>
       </c>
-      <c r="W5">
-        <v>-1.05191082665109</v>
-      </c>
       <c r="X5">
-        <v>-0.853645217176353</v>
+        <v>-0.897201725003773</v>
       </c>
       <c r="Y5">
-        <v>0.487905759876115</v>
+        <v>-0.581448875082744</v>
       </c>
       <c r="Z5">
+        <v>0.506036927659891</v>
+      </c>
+      <c r="AA5">
         <v>0.00878987146533087</v>
       </c>
-      <c r="AA5">
-        <v>-0.144898012301384</v>
+      <c r="AB5">
+        <v>0.138859233081572</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:28">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>0.2</v>
@@ -1013,7 +1031,7 @@
         <v>0.166666666666667</v>
       </c>
       <c r="E6">
-        <v>0.32866964087565</v>
+        <v>4.62592926927149e-17</v>
       </c>
       <c r="F6">
         <v>0.277684053800249</v>
@@ -1061,30 +1079,33 @@
         <v>1.70348091513135</v>
       </c>
       <c r="U6">
+        <v>1.00469437491623</v>
+      </c>
+      <c r="V6">
         <v>1.47877966604166</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>0.866025403784439</v>
       </c>
-      <c r="W6">
-        <v>1.69741990976954</v>
-      </c>
       <c r="X6">
-        <v>0.614796557862919</v>
+        <v>0.488559381720309</v>
       </c>
       <c r="Y6">
-        <v>1.31832895468212</v>
+        <v>0.485109973593671</v>
       </c>
       <c r="Z6">
+        <v>1.26762472216491</v>
+      </c>
+      <c r="AA6">
         <v>0.0124307554377872</v>
       </c>
-      <c r="AA6">
-        <v>0.263660888901169</v>
+      <c r="AB6">
+        <v>0.0141810699862672</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:28">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -1144,30 +1165,33 @@
         <v>2.71409499247695</v>
       </c>
       <c r="U7">
+        <v>2.10987192594582</v>
+      </c>
+      <c r="V7">
         <v>0.99046817359701</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>0.774596669241483</v>
       </c>
-      <c r="W7">
-        <v>-1.69741990976954</v>
-      </c>
       <c r="X7">
-        <v>0.270097535571253</v>
+        <v>-0.488559381720309</v>
       </c>
       <c r="Y7">
-        <v>0.75853602126271</v>
+        <v>-0.518911059921971</v>
       </c>
       <c r="Z7">
+        <v>0.788877009508105</v>
+      </c>
+      <c r="AA7">
         <v>0.0124307554377872</v>
       </c>
-      <c r="AA7">
-        <v>-0.206038554769815</v>
+      <c r="AB7">
+        <v>0.0450613939023632</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:28">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>0.120879120879121</v>
@@ -1194,7 +1218,7 @@
         <v>0.462244897959184</v>
       </c>
       <c r="J8">
-        <v>0.28844474056596</v>
+        <v>0.288444740565959</v>
       </c>
       <c r="K8">
         <v>-0.170820396579082</v>
@@ -1227,30 +1251,33 @@
         <v>1.13613234829841</v>
       </c>
       <c r="U8">
+        <v>0.521753071433778</v>
+      </c>
+      <c r="V8">
         <v>2.99976016185179</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>0.875199449684285</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>1.04529271084357</v>
       </c>
-      <c r="X8">
-        <v>1.22434314905709</v>
-      </c>
       <c r="Y8">
-        <v>2.01279597217926</v>
+        <v>0.811771565644955</v>
       </c>
       <c r="Z8">
+        <v>2.31444824464738</v>
+      </c>
+      <c r="AA8">
         <v>0.0070118917343666</v>
       </c>
-      <c r="AA8">
-        <v>0.186687152903642</v>
+      <c r="AB8">
+        <v>0.0175355147402597</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:28">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>0.0661764705882353</v>
@@ -1310,30 +1337,33 @@
         <v>2.06482289797069</v>
       </c>
       <c r="U9">
+        <v>0.51425975821474</v>
+      </c>
+      <c r="V9">
         <v>1.85851850115771</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>0.807135917344422</v>
       </c>
-      <c r="W9">
-        <v>14.0709202030539</v>
-      </c>
       <c r="X9">
-        <v>1.78523177094415</v>
+        <v>14.2035235053185</v>
       </c>
       <c r="Y9">
-        <v>0.908884467951915</v>
+        <v>0.47246690832198</v>
       </c>
       <c r="Z9">
+        <v>0.808652281774728</v>
+      </c>
+      <c r="AA9">
         <v>0.0145159949751711</v>
       </c>
-      <c r="AA9">
-        <v>0.47136943766907</v>
+      <c r="AB9">
+        <v>0.436430033233274</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:28">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>0.0947712418300654</v>
@@ -1378,7 +1408,7 @@
         <v>0.0012197536997668</v>
       </c>
       <c r="P10">
-        <v>-0.0019606400934367</v>
+        <v>-0.00196064009343671</v>
       </c>
       <c r="Q10">
         <v>0.0351036320366731</v>
@@ -1393,30 +1423,33 @@
         <v>0.867579908342579</v>
       </c>
       <c r="U10">
-        <v>3.27908465014459</v>
+        <v>0.39099210247442</v>
       </c>
       <c r="V10">
+        <v>3.27908465014458</v>
+      </c>
+      <c r="W10">
         <v>0.877326717582169</v>
       </c>
-      <c r="W10">
-        <v>-13.6340352261333</v>
-      </c>
       <c r="X10">
-        <v>-1.00281087588735</v>
+        <v>-13.7666385283979</v>
       </c>
       <c r="Y10">
-        <v>1.72134344587126</v>
+        <v>-2.01265121926743</v>
       </c>
       <c r="Z10">
+        <v>1.67478901222027</v>
+      </c>
+      <c r="AA10">
         <v>0.0131379693689775</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:28">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>0.0887445887445887</v>
@@ -1428,7 +1461,7 @@
         <v>0.0571428571428571</v>
       </c>
       <c r="E11">
-        <v>0.14296285615201</v>
+        <v>0.154598055827368</v>
       </c>
       <c r="F11">
         <v>0.183911998623885</v>
@@ -1476,30 +1509,33 @@
         <v>1.56458947739323</v>
       </c>
       <c r="U11">
+        <v>0.339003050587286</v>
+      </c>
+      <c r="V11">
         <v>2.64665190728862</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>0.866815032280218</v>
       </c>
-      <c r="W11">
-        <v>-0.192578685742613</v>
-      </c>
       <c r="X11">
-        <v>0.766294317803198</v>
+        <v>-0.192578685742593</v>
       </c>
       <c r="Y11">
-        <v>0.817432300754284</v>
+        <v>0.433787786735178</v>
       </c>
       <c r="Z11">
+        <v>0.777286658254289</v>
+      </c>
+      <c r="AA11">
         <v>0.0150361523392413</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:28">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>0.0711462450592885</v>
@@ -1526,7 +1562,7 @@
         <v>0.311242863416776</v>
       </c>
       <c r="J12">
-        <v>0.159162627197141</v>
+        <v>0.159162627197142</v>
       </c>
       <c r="K12">
         <v>-0.196526804855736</v>
@@ -1544,7 +1580,7 @@
         <v>0.000937584186792267</v>
       </c>
       <c r="P12">
-        <v>-0.000271422356818972</v>
+        <v>-0.000271422356818971</v>
       </c>
       <c r="Q12">
         <v>-0.0589987343165555</v>
@@ -1559,30 +1595,33 @@
         <v>0.873609664017829</v>
       </c>
       <c r="U12">
-        <v>3.60129484592719</v>
+        <v>0.383853435594322</v>
       </c>
       <c r="V12">
+        <v>3.60129484592718</v>
+      </c>
+      <c r="W12">
         <v>0.864472116206825</v>
       </c>
-      <c r="W12">
-        <v>1.0337269710037</v>
-      </c>
       <c r="X12">
-        <v>0.576757883719376</v>
+        <v>1.03372697100383</v>
       </c>
       <c r="Y12">
-        <v>1.22070400001624</v>
+        <v>0.652177322372871</v>
       </c>
       <c r="Z12">
+        <v>1.26413840366728</v>
+      </c>
+      <c r="AA12">
         <v>0.0140866989190509</v>
       </c>
-      <c r="AA12">
-        <v>0.207610035607276</v>
+      <c r="AB12">
+        <v>0.245113874367292</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:28">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>0.0707692307692308</v>
@@ -1594,7 +1633,7 @@
         <v>0.0288034188034188</v>
       </c>
       <c r="E13">
-        <v>0.127862044081464</v>
+        <v>0.132363137816978</v>
       </c>
       <c r="F13">
         <v>0.17244723549779</v>
@@ -1636,36 +1675,39 @@
         <v>0.24206070582967</v>
       </c>
       <c r="S13">
-        <v>0.00918503072751308</v>
+        <v>0.0091850307275131</v>
       </c>
       <c r="T13">
         <v>1.94223309670409</v>
       </c>
       <c r="U13">
+        <v>0.317377910646316</v>
+      </c>
+      <c r="V13">
         <v>2.30044561405935</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>0.882611041995053</v>
       </c>
-      <c r="W13">
-        <v>-1.63461113465214</v>
-      </c>
       <c r="X13">
-        <v>-1.18834813707523</v>
+        <v>-1.63461113465225</v>
       </c>
       <c r="Y13">
-        <v>1.26845788294828</v>
+        <v>-1.23324770649182</v>
       </c>
       <c r="Z13">
+        <v>1.11245614660158</v>
+      </c>
+      <c r="AA13">
         <v>0.0154534567266276</v>
       </c>
-      <c r="AA13">
-        <v>-0.504563175973437</v>
+      <c r="AB13">
+        <v>-0.515990604259365</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:28">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>0.0857142857142857</v>
@@ -1677,7 +1719,7 @@
         <v>0.0511278195488722</v>
       </c>
       <c r="E14">
-        <v>0.147848044117481</v>
+        <v>0.134181329316739</v>
       </c>
       <c r="F14">
         <v>0.194930973777029</v>
@@ -1707,10 +1749,10 @@
         <v>0.0260732122901997</v>
       </c>
       <c r="O14">
-        <v>0.00153946641530762</v>
+        <v>0.00153946641530761</v>
       </c>
       <c r="P14">
-        <v>0.00316977639007487</v>
+        <v>0.00316977639007486</v>
       </c>
       <c r="Q14">
         <v>-0.0351738994298548</v>
@@ -1725,30 +1767,33 @@
         <v>2.88826893497679</v>
       </c>
       <c r="U14">
+        <v>0.385057103563361</v>
+      </c>
+      <c r="V14">
         <v>2.40865514191426</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>0.868312685532289</v>
       </c>
-      <c r="W14">
-        <v>2.22407908330382</v>
-      </c>
       <c r="X14">
-        <v>-0.306078378431768</v>
+        <v>2.22407908330415</v>
       </c>
       <c r="Y14">
-        <v>0.603924264107491</v>
+        <v>-0.522392944942876</v>
       </c>
       <c r="Z14">
+        <v>0.670956461095335</v>
+      </c>
+      <c r="AA14">
         <v>0.0160828854606541</v>
       </c>
-      <c r="AA14">
-        <v>0.508278477296733</v>
+      <c r="AB14">
+        <v>0.507210001626856</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:28">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>0.0256892230576441</v>
@@ -1760,7 +1805,7 @@
         <v>0.0388357256778309</v>
       </c>
       <c r="E15">
-        <v>0.0696624296349748</v>
+        <v>0.0696200406283525</v>
       </c>
       <c r="F15">
         <v>0.106213076196652</v>
@@ -1808,30 +1853,33 @@
         <v>-0.47246324086553</v>
       </c>
       <c r="U15">
-        <v>3.91014917138463</v>
+        <v>0.173522401179611</v>
       </c>
       <c r="V15">
+        <v>3.91014917138464</v>
+      </c>
+      <c r="W15">
         <v>0.886019297085595</v>
       </c>
-      <c r="W15">
-        <v>0.700871081985116</v>
-      </c>
       <c r="X15">
-        <v>1.38816303780057</v>
+        <v>0.700871081987218</v>
       </c>
       <c r="Y15">
-        <v>3.47512635591994</v>
+        <v>1.31020972411758</v>
       </c>
       <c r="Z15">
+        <v>1.9831463476176</v>
+      </c>
+      <c r="AA15">
         <v>0.0113929755478287</v>
       </c>
-      <c r="AA15">
-        <v>0.0202201338050722</v>
+      <c r="AB15">
+        <v>-0.126806144606597</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:28">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>0.0223776223776224</v>
@@ -1843,10 +1891,10 @@
         <v>0.0349478126040626</v>
       </c>
       <c r="E16">
-        <v>0.0669982594194598</v>
+        <v>0.0693713422359863</v>
       </c>
       <c r="F16">
-        <v>0.0995557405453889</v>
+        <v>0.0970862771987126</v>
       </c>
       <c r="G16">
         <v>0.0349509366501554</v>
@@ -1891,30 +1939,33 @@
         <v>0.559209850154011</v>
       </c>
       <c r="U16">
+        <v>0.154447087560937</v>
+      </c>
+      <c r="V16">
         <v>3.99559473284366</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>0.874580664789574</v>
       </c>
-      <c r="W16">
-        <v>-2.8331062521871</v>
-      </c>
       <c r="X16">
-        <v>-0.979063228217563</v>
+        <v>-2.83310625218948</v>
       </c>
       <c r="Y16">
-        <v>0.648501521447253</v>
+        <v>-0.822708844046067</v>
       </c>
       <c r="Z16">
+        <v>1.20154532247878</v>
+      </c>
+      <c r="AA16">
         <v>0.0145604426441847</v>
       </c>
-      <c r="AA16">
-        <v>-0.71971545076833</v>
+      <c r="AB16">
+        <v>-0.589142096510315</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:28">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>0.0266257040450589</v>
@@ -1926,7 +1977,7 @@
         <v>0.0353255645051369</v>
       </c>
       <c r="E17">
-        <v>0.0843351358953168</v>
+        <v>0.0828246484585054</v>
       </c>
       <c r="F17">
         <v>0.104651531925811</v>
@@ -1974,30 +2025,33 @@
         <v>1.39659784307366</v>
       </c>
       <c r="U17">
+        <v>0.148491327021749</v>
+      </c>
+      <c r="V17">
         <v>3.59628811091275</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>0.906442057572407</v>
       </c>
-      <c r="W17">
-        <v>1.17264436501075</v>
-      </c>
       <c r="X17">
-        <v>-0.285897814894531</v>
+        <v>1.17264436501067</v>
       </c>
       <c r="Y17">
-        <v>0.986712034676278</v>
+        <v>-0.666405340177337</v>
       </c>
       <c r="Z17">
+        <v>0.924802671300506</v>
+      </c>
+      <c r="AA17">
         <v>0.014825334134991</v>
       </c>
-      <c r="AA17">
-        <v>0.655269943305426</v>
+      <c r="AB17">
+        <v>0.543712152452201</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:28">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>0.014809329877823</v>
@@ -2009,10 +2063,10 @@
         <v>0.0465311201612571</v>
       </c>
       <c r="E18">
-        <v>0.0650027797097374</v>
+        <v>0.0650027797097375</v>
       </c>
       <c r="F18">
-        <v>0.0973542790063602</v>
+        <v>0.0983420077274808</v>
       </c>
       <c r="G18">
         <v>0.0465311201612572</v>
@@ -2024,7 +2078,7 @@
         <v>0.235756360756361</v>
       </c>
       <c r="J18">
-        <v>0.0646489545249885</v>
+        <v>0.0646489545249864</v>
       </c>
       <c r="K18">
         <v>-0.237276142988631</v>
@@ -2039,7 +2093,7 @@
         <v>0.00229428000061773</v>
       </c>
       <c r="O18">
-        <v>0.000770633427730446</v>
+        <v>0.000770633427730445</v>
       </c>
       <c r="P18">
         <v>-0.000582474384166742</v>
@@ -2057,30 +2111,33 @@
         <v>-0.285604834389905</v>
       </c>
       <c r="U18">
-        <v>5.36382157674723</v>
+        <v>0.133707028717612</v>
       </c>
       <c r="V18">
+        <v>5.36382157674724</v>
+      </c>
+      <c r="W18">
         <v>0.890153580267585</v>
       </c>
-      <c r="W18">
-        <v>-0.246935913586076</v>
-      </c>
       <c r="X18">
-        <v>-1.08268963872178</v>
+        <v>-0.246935913586046</v>
       </c>
       <c r="Y18">
-        <v>1.15017241711094</v>
+        <v>-1.76735249131819</v>
       </c>
       <c r="Z18">
+        <v>1.15043757269209</v>
+      </c>
+      <c r="AA18">
         <v>0.0153540765528727</v>
       </c>
-      <c r="AA18">
-        <v>-0.248977703341267</v>
+      <c r="AB18">
+        <v>-0.286852095566334</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:28">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19">
         <v>0.0104642313546423</v>
@@ -2092,10 +2149,10 @@
         <v>0.0422642399296846</v>
       </c>
       <c r="E19">
-        <v>0.053698032906832</v>
+        <v>0.0536980329068273</v>
       </c>
       <c r="F19">
-        <v>0.103359082534663</v>
+        <v>0.103244650763905</v>
       </c>
       <c r="G19">
         <v>0.0422642399296847</v>
@@ -2122,7 +2179,7 @@
         <v>-0.0041274550123702</v>
       </c>
       <c r="O19">
-        <v>0.000308610129900834</v>
+        <v>0.000308610129900835</v>
       </c>
       <c r="P19">
         <v>0.00181615696146753</v>
@@ -2140,30 +2197,33 @@
         <v>2.98868154159287</v>
       </c>
       <c r="U19">
-        <v>6.43388816542624</v>
+        <v>0.153779670487269</v>
       </c>
       <c r="V19">
+        <v>6.43388816542621</v>
+      </c>
+      <c r="W19">
         <v>0.860997637027291</v>
       </c>
-      <c r="W19">
-        <v>-0.370739975058558</v>
-      </c>
       <c r="X19">
-        <v>2.41117600821318</v>
+        <v>0.267763637933634</v>
       </c>
       <c r="Y19">
-        <v>1.06896439663969</v>
+        <v>0.0174051951199651</v>
       </c>
       <c r="Z19">
+        <v>1.21194834513487</v>
+      </c>
+      <c r="AA19">
         <v>0.0158764726629214</v>
       </c>
-      <c r="AA19">
-        <v>0.524839242191961</v>
+      <c r="AB19">
+        <v>0.513540079091851</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:28">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20">
         <v>0.0140350877192982</v>
@@ -2175,10 +2235,10 @@
         <v>0.0330912754860123</v>
       </c>
       <c r="E20">
-        <v>0.0714575293344729</v>
+        <v>0.072435091637446</v>
       </c>
       <c r="F20">
-        <v>0.104187684027673</v>
+        <v>0.106258330785552</v>
       </c>
       <c r="G20">
         <v>0.0330894051946684</v>
@@ -2223,30 +2283,33 @@
         <v>-0.243878494774433</v>
       </c>
       <c r="U20">
-        <v>3.99088824392554</v>
+        <v>0.138612698821634</v>
       </c>
       <c r="V20">
+        <v>3.99088824392553</v>
+      </c>
+      <c r="W20">
         <v>0.884417516687752</v>
       </c>
-      <c r="W20">
-        <v>1.05075613713745</v>
-      </c>
       <c r="X20">
-        <v>1.40976557261538</v>
+        <v>0.412252524144743</v>
       </c>
       <c r="Y20">
-        <v>0.907380390841924</v>
+        <v>2.21238099527125</v>
       </c>
       <c r="Z20">
+        <v>0.857412349504984</v>
+      </c>
+      <c r="AA20">
         <v>0.0141937749294579</v>
       </c>
-      <c r="AA20">
-        <v>-0.367113848097586</v>
+      <c r="AB20">
+        <v>-0.274203165509894</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:28">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B21">
         <v>0.0108669108669109</v>
@@ -2258,7 +2321,7 @@
         <v>0.0278772413603874</v>
       </c>
       <c r="E21">
-        <v>0.0685023667932585</v>
+        <v>0.0685023667932586</v>
       </c>
       <c r="F21">
         <v>0.0912098343907094</v>
@@ -2306,30 +2369,33 @@
         <v>1.59470545332285</v>
       </c>
       <c r="U21">
+        <v>0.121188938722717</v>
+      </c>
+      <c r="V21">
         <v>3.46593592744942</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>0.883580622264781</v>
       </c>
-      <c r="W21">
-        <v>1.145740474131</v>
-      </c>
       <c r="X21">
-        <v>0.562431634653335</v>
+        <v>1.14574047413131</v>
       </c>
       <c r="Y21">
-        <v>0.993876622141327</v>
+        <v>1.17045410648057</v>
       </c>
       <c r="Z21">
+        <v>1.00021621189333</v>
+      </c>
+      <c r="AA21">
         <v>0.0145117123390032</v>
       </c>
-      <c r="AA21">
-        <v>0.0495124643559382</v>
+      <c r="AB21">
+        <v>0.0931650791547288</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:28">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22">
         <v>0.012697323266987</v>
@@ -2341,10 +2407,10 @@
         <v>0.0267869971306903</v>
       </c>
       <c r="E22">
-        <v>0.0683111177551116</v>
+        <v>0.0682675509441143</v>
       </c>
       <c r="F22">
-        <v>0.0860935286033843</v>
+        <v>0.0855899035511182</v>
       </c>
       <c r="G22">
         <v>0.0267849963859297</v>
@@ -2374,7 +2440,7 @@
         <v>0.000957671523664443</v>
       </c>
       <c r="P22">
-        <v>-0.000770937503635759</v>
+        <v>-0.00077093750363576</v>
       </c>
       <c r="Q22">
         <v>0.00344033090538006</v>
@@ -2389,30 +2455,33 @@
         <v>3.2675269361724</v>
       </c>
       <c r="U22">
+        <v>0.108410878517458</v>
+      </c>
+      <c r="V22">
         <v>3.20554070036015</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>0.906075454707446</v>
       </c>
-      <c r="W22">
-        <v>-1.50978661909184</v>
-      </c>
       <c r="X22">
-        <v>0.439728819521156</v>
+        <v>-1.50978661909173</v>
       </c>
       <c r="Y22">
-        <v>1.14969210902986</v>
+        <v>-1.7271672013762</v>
       </c>
       <c r="Z22">
+        <v>1.08262677035413</v>
+      </c>
+      <c r="AA22">
         <v>0.014594047644061</v>
       </c>
-      <c r="AA22">
-        <v>-0.0658626360806904</v>
+      <c r="AB22">
+        <v>-0.342867141409779</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:28">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>0.0165137614678899</v>
@@ -2424,10 +2493,10 @@
         <v>0.017814682061624</v>
       </c>
       <c r="E23">
-        <v>0.0633610614551491</v>
+        <v>0.062979172016208</v>
       </c>
       <c r="F23">
-        <v>0.0684365807313087</v>
+        <v>0.0693270581566532</v>
       </c>
       <c r="G23">
         <v>0.0178144179036126</v>
@@ -2448,54 +2517,57 @@
         <v>0.216864362850934</v>
       </c>
       <c r="M23">
-        <v>-0.0172667504772496</v>
+        <v>0.00129720611214465</v>
       </c>
       <c r="N23">
-        <v>0.00135057574206262</v>
+        <v>-0.000337056675155041</v>
       </c>
       <c r="O23">
         <v>0.00068200509311711</v>
       </c>
       <c r="P23">
-        <v>-0.000409349390446451</v>
+        <v>-0.000409349390446452</v>
       </c>
       <c r="Q23">
-        <v>0.0019604700279352</v>
+        <v>0.000954381471516984</v>
       </c>
       <c r="R23">
-        <v>0.0599470991942968</v>
+        <v>0.0593685867976025</v>
       </c>
       <c r="S23">
-        <v>0.030085174546529</v>
+        <v>-0.0145209383957365</v>
       </c>
       <c r="T23">
-        <v>-0.40633790080587</v>
+        <v>0.027077551541747</v>
       </c>
       <c r="U23">
+        <v>0.0925563413168103</v>
+      </c>
+      <c r="V23">
         <v>2.79120281224702</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>0.919218457148041</v>
       </c>
-      <c r="W23">
-        <v>1.12579431337031</v>
-      </c>
       <c r="X23">
-        <v>-1.41525850893781</v>
+        <v>1.12579431337032</v>
       </c>
       <c r="Y23">
-        <v>0.823466610119958</v>
+        <v>1.36737427802183</v>
       </c>
       <c r="Z23">
+        <v>0.843191566922032</v>
+      </c>
+      <c r="AA23">
         <v>0.014389861392556</v>
       </c>
-      <c r="AA23">
-        <v>-0.459535599239836</v>
+      <c r="AB23">
+        <v>0.171534251732725</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:28">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>0.0121474685694869</v>
@@ -2507,10 +2579,10 @@
         <v>0.0194173148347547</v>
       </c>
       <c r="E24">
-        <v>0.0620148193059091</v>
+        <v>0.0620148193059092</v>
       </c>
       <c r="F24">
-        <v>0.0737468264816389</v>
+        <v>0.0732996395206396</v>
       </c>
       <c r="G24">
         <v>0.0194173516609576</v>
@@ -2555,30 +2627,33 @@
         <v>0.479904588516142</v>
       </c>
       <c r="U24">
+        <v>0.0972055703052011</v>
+      </c>
+      <c r="V24">
         <v>3.04697053345346</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>0.902101413567922</v>
       </c>
-      <c r="W24">
-        <v>-0.541538212690746</v>
-      </c>
       <c r="X24">
-        <v>-2.70338416780498</v>
+        <v>-0.541538212692925</v>
       </c>
       <c r="Y24">
-        <v>6.36640412963768</v>
+        <v>-0.853489396564862</v>
       </c>
       <c r="Z24">
+        <v>7.76865635718985</v>
+      </c>
+      <c r="AA24">
         <v>0.0161524545736765</v>
       </c>
-      <c r="AA24">
-        <v>0.455185284677532</v>
+      <c r="AB24">
+        <v>0.333067720923528</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:28">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>0.018085842852198</v>
@@ -2623,7 +2698,7 @@
         <v>-0.000628119921765591</v>
       </c>
       <c r="P25">
-        <v>2.91084213109642e-05</v>
+        <v>2.9108421310964e-05</v>
       </c>
       <c r="Q25">
         <v>-0.00232726284882278</v>
@@ -2638,30 +2713,33 @@
         <v>0.825007946136305</v>
       </c>
       <c r="U25">
+        <v>0.0907831382949899</v>
+      </c>
+      <c r="V25">
         <v>2.89053231611236</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>0.918644292746289</v>
       </c>
-      <c r="W25">
-        <v>-0.40115131886765</v>
-      </c>
       <c r="X25">
-        <v>0.354501699724576</v>
+        <v>-0.401151318866104</v>
       </c>
       <c r="Y25">
-        <v>0.158850872775147</v>
+        <v>1.26530472847503</v>
       </c>
       <c r="Z25">
+        <v>0.12923718592526</v>
+      </c>
+      <c r="AA25">
         <v>0.0153914881537371</v>
       </c>
-      <c r="AA25">
-        <v>-0.3333077950483</v>
+      <c r="AB25">
+        <v>-0.437685153528964</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:28">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>0.0108838185156045</v>
@@ -2673,10 +2751,10 @@
         <v>0.0177885834913347</v>
       </c>
       <c r="E26">
-        <v>0.0546613673021631</v>
+        <v>0.0541939222499953</v>
       </c>
       <c r="F26">
-        <v>0.0586200737823094</v>
+        <v>0.0587299956992259</v>
       </c>
       <c r="G26">
         <v>0.0177885834913346</v>
@@ -2706,7 +2784,7 @@
         <v>-0.000543599765062118</v>
       </c>
       <c r="P26">
-        <v>-0.000478545884941443</v>
+        <v>-0.000478545884941442</v>
       </c>
       <c r="Q26">
         <v>-0.0020268346135824</v>
@@ -2721,30 +2799,33 @@
         <v>-0.010548687411952</v>
       </c>
       <c r="U26">
+        <v>0.0846765204506203</v>
+      </c>
+      <c r="V26">
         <v>3.41931170020565</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>0.906208256156452</v>
       </c>
-      <c r="W26">
-        <v>0.0650015997574016</v>
-      </c>
       <c r="X26">
-        <v>-1.49678311568755</v>
+        <v>0.0503465735170285</v>
       </c>
       <c r="Y26">
-        <v>2.31070909967728</v>
+        <v>-1.50257940114557</v>
       </c>
       <c r="Z26">
+        <v>2.31622776483311</v>
+      </c>
+      <c r="AA26">
         <v>0.0157083458970645</v>
       </c>
-      <c r="AA26">
-        <v>0.0221415726462084</v>
+      <c r="AB26">
+        <v>-0.113489176287941</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:28">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>0.013886910696482</v>
@@ -2756,10 +2837,10 @@
         <v>0.0191988138149654</v>
       </c>
       <c r="E27">
-        <v>0.051451015901696</v>
+        <v>0.0514510159016959</v>
       </c>
       <c r="F27">
-        <v>0.0389426665588692</v>
+        <v>0.0389465104958087</v>
       </c>
       <c r="G27">
         <v>0.0191988138149654</v>
@@ -2780,10 +2861,10 @@
         <v>0.212814006867601</v>
       </c>
       <c r="M27">
-        <v>0.0468805716548063</v>
+        <v>0.0487662815309106</v>
       </c>
       <c r="N27">
-        <v>-0.000693271324243439</v>
+        <v>-0.000360498993166206</v>
       </c>
       <c r="O27">
         <v>-0.00137926356270731</v>
@@ -2792,42 +2873,45 @@
         <v>-0.000537535978567043</v>
       </c>
       <c r="Q27">
-        <v>-0.000605183560490364</v>
+        <v>-0.000882493836388059</v>
       </c>
       <c r="R27">
-        <v>0.0607968593536576</v>
+        <v>0.0608674758355445</v>
       </c>
       <c r="S27">
-        <v>-0.0275244328985548</v>
+        <v>-0.018475515430086</v>
       </c>
       <c r="T27">
-        <v>1.19862504872148</v>
+        <v>1.24817579802182</v>
       </c>
       <c r="U27">
-        <v>3.52066171800198</v>
+        <v>0.0875586154166511</v>
       </c>
       <c r="V27">
+        <v>3.52066171800199</v>
+      </c>
+      <c r="W27">
         <v>0.911104447221316</v>
       </c>
-      <c r="W27">
-        <v>-0.141684921779725</v>
-      </c>
       <c r="X27">
-        <v>1.38151543494553</v>
+        <v>-0.127029895539097</v>
       </c>
       <c r="Y27">
-        <v>0.487947303386618</v>
+        <v>-0.324444622645889</v>
       </c>
       <c r="Z27">
+        <v>0.476635904538478</v>
+      </c>
+      <c r="AA27">
         <v>0.0154573970921823</v>
       </c>
-      <c r="AA27">
-        <v>0.273807624878081</v>
+      <c r="AB27">
+        <v>0.0933900274982669</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:28">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>0.0131785995279308</v>
@@ -2842,7 +2926,7 @@
         <v>0.0551698745630715</v>
       </c>
       <c r="F28">
-        <v>0.0482438407278875</v>
+        <v>0.0481767022283596</v>
       </c>
       <c r="G28">
         <v>0.0177101202529741</v>
@@ -2872,7 +2956,7 @@
         <v>-0.000668052040469291</v>
       </c>
       <c r="P28">
-        <v>0.000260754853689388</v>
+        <v>0.000260754853689389</v>
       </c>
       <c r="Q28">
         <v>0.00317089695816674</v>
@@ -2887,30 +2971,33 @@
         <v>-0.0168650889539627</v>
       </c>
       <c r="U28">
-        <v>3.15863502856579</v>
+        <v>0.0841020445758814</v>
       </c>
       <c r="V28">
+        <v>3.1586350285658</v>
+      </c>
+      <c r="W28">
         <v>0.918795853622625</v>
       </c>
-      <c r="W28">
-        <v>-0.491368424547045</v>
-      </c>
       <c r="X28">
-        <v>0.154986937700053</v>
+        <v>-0.491368424546479</v>
       </c>
       <c r="Y28">
-        <v>0.938555672609553</v>
+        <v>-0.37551045584544</v>
       </c>
       <c r="Z28">
+        <v>0.960949684158334</v>
+      </c>
+      <c r="AA28">
         <v>0.0159509673976893</v>
       </c>
-      <c r="AA28">
-        <v>-0.329200170677304</v>
+      <c r="AB28">
+        <v>-0.236048285779486</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:28">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B29">
         <v>0.0120518688024409</v>
@@ -2922,10 +3009,10 @@
         <v>0.0218669203863541</v>
       </c>
       <c r="E29">
-        <v>0.0646855661853243</v>
+        <v>0.0646928351282232</v>
       </c>
       <c r="F29">
-        <v>0.074620180597347</v>
+        <v>0.0745568173055648</v>
       </c>
       <c r="G29">
         <v>0.0218670087624831</v>
@@ -2946,54 +3033,57 @@
         <v>0.219950283262223</v>
       </c>
       <c r="M29">
-        <v>-0.0502300751573509</v>
+        <v>-0.0587818585622078</v>
       </c>
       <c r="N29">
-        <v>-0.002250190606349</v>
+        <v>0.000362854322912831</v>
       </c>
       <c r="O29">
-        <v>-0.000726808021595738</v>
+        <v>-0.000726808021595739</v>
       </c>
       <c r="P29">
-        <v>-0.000959535077172782</v>
+        <v>-0.000959535077172781</v>
       </c>
       <c r="Q29">
-        <v>0.00535224004220277</v>
+        <v>0.00645090666018786</v>
       </c>
       <c r="R29">
         <v>0.05267927586099</v>
       </c>
       <c r="S29">
-        <v>-0.0613853594063631</v>
+        <v>-0.0113934096288591</v>
       </c>
       <c r="T29">
-        <v>-1.2637015952273</v>
+        <v>-1.48339094038488</v>
       </c>
       <c r="U29">
-        <v>3.61397596517137</v>
+        <v>0.0922456122497239</v>
       </c>
       <c r="V29">
+        <v>3.61397596517136</v>
+      </c>
+      <c r="W29">
         <v>0.914105246860338</v>
       </c>
-      <c r="W29">
-        <v>-0.225297129925138</v>
-      </c>
       <c r="X29">
-        <v>-0.934557070631527</v>
+        <v>-0.225297129925249</v>
       </c>
       <c r="Y29">
-        <v>1.19335042512633</v>
+        <v>0.417301001920751</v>
       </c>
       <c r="Z29">
+        <v>1.14105994136533</v>
+      </c>
+      <c r="AA29">
         <v>0.0163705868910213</v>
       </c>
-      <c r="AA29">
-        <v>-0.264164328800264</v>
+      <c r="AB29">
+        <v>0.0359112870243731</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:28">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B30">
         <v>0.0129819040125885</v>
@@ -3005,10 +3095,10 @@
         <v>0.0175248267621899</v>
       </c>
       <c r="E30">
-        <v>0.0587941074784044</v>
+        <v>0.0585471689615329</v>
       </c>
       <c r="F30">
-        <v>0.0573386507422087</v>
+        <v>0.0571860152749577</v>
       </c>
       <c r="G30">
         <v>0.0175266027101704</v>
@@ -3035,7 +3125,7 @@
         <v>0.00247360909229837</v>
       </c>
       <c r="O30">
-        <v>-0.000253911235636766</v>
+        <v>-0.000253911235636765</v>
       </c>
       <c r="P30">
         <v>0.000573863038903924</v>
@@ -3053,30 +3143,33 @@
         <v>0.219601621426497</v>
       </c>
       <c r="U30">
+        <v>0.0826588343858754</v>
+      </c>
+      <c r="V30">
         <v>3.04533528674403</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>0.920765432702475</v>
       </c>
-      <c r="W30">
-        <v>0.227354792574308</v>
-      </c>
       <c r="X30">
-        <v>0.139227600919719</v>
+        <v>0.227354792574418</v>
       </c>
       <c r="Y30">
-        <v>0.946094252235949</v>
+        <v>1.80784665677357</v>
       </c>
       <c r="Z30">
+        <v>0.903122873636587</v>
+      </c>
+      <c r="AA30">
         <v>0.0156018477241692</v>
       </c>
-      <c r="AA30">
-        <v>0.362055877466574</v>
+      <c r="AB30">
+        <v>0.3461946926017</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:28">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31">
         <v>0.0156071998177261</v>
@@ -3088,10 +3181,10 @@
         <v>0.0179282348828351</v>
       </c>
       <c r="E31">
-        <v>0.0519141811073833</v>
+        <v>0.0519141811073832</v>
       </c>
       <c r="F31">
-        <v>0.00299546276384042</v>
+        <v>0.00302772907686889</v>
       </c>
       <c r="G31">
         <v>0.0179282348828351</v>
@@ -3118,7 +3211,7 @@
         <v>-5.69613192794711e-06</v>
       </c>
       <c r="O31">
-        <v>0.000195140638252579</v>
+        <v>0.00019514063825258</v>
       </c>
       <c r="P31">
         <v>0.000355765912549851</v>
@@ -3130,36 +3223,39 @@
         <v>0.0427988696544067</v>
       </c>
       <c r="S31">
-        <v>-0.00858531383938013</v>
+        <v>-0.00858531383938014</v>
       </c>
       <c r="T31">
         <v>-0.196085918974164</v>
       </c>
       <c r="U31">
+        <v>0.0806787761306662</v>
+      </c>
+      <c r="V31">
         <v>3.07962983421652</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>0.921753188231864</v>
       </c>
-      <c r="W31">
-        <v>1.30380508791649</v>
-      </c>
       <c r="X31">
-        <v>-0.828633894425627</v>
+        <v>1.30380508791589</v>
       </c>
       <c r="Y31">
-        <v>0.904090206526913</v>
+        <v>0.254549279559754</v>
       </c>
       <c r="Z31">
+        <v>1.04754649712551</v>
+      </c>
+      <c r="AA31">
         <v>0.0155941129759143</v>
       </c>
-      <c r="AA31">
-        <v>-0.067430633608431</v>
+      <c r="AB31">
+        <v>-0.102886312182736</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:28">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B32">
         <v>0.0124005027230834</v>
@@ -3171,7 +3267,7 @@
         <v>0.0115482368474337</v>
       </c>
       <c r="E32">
-        <v>0.0529949940828381</v>
+        <v>0.0530213931816469</v>
       </c>
       <c r="F32">
         <v>0.0221077853966976</v>
@@ -3195,54 +3291,57 @@
         <v>0.182735639150944</v>
       </c>
       <c r="M32">
-        <v>-0.000566502642629996</v>
+        <v>-0.000566502642629998</v>
       </c>
       <c r="N32">
-        <v>0.0015489179484145</v>
+        <v>0.00279117102683711</v>
       </c>
       <c r="O32">
-        <v>-0.000206835330696453</v>
+        <v>-0.000206835330696454</v>
       </c>
       <c r="P32">
-        <v>-0.000119473697315765</v>
+        <v>-0.000119473697315764</v>
       </c>
       <c r="Q32">
-        <v>0.000935022888260413</v>
+        <v>-1.30123557989417e-05</v>
       </c>
       <c r="R32">
-        <v>0.0417187394197838</v>
+        <v>0.0415522461835715</v>
       </c>
       <c r="S32">
-        <v>0.0442747293255571</v>
+        <v>0.0773628633013401</v>
       </c>
       <c r="T32">
-        <v>-0.0591637155308961</v>
+        <v>-0.0545894903096879</v>
       </c>
       <c r="U32">
+        <v>0.0672026085692898</v>
+      </c>
+      <c r="V32">
         <v>2.78185191994785</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <v>0.932925077025979</v>
       </c>
-      <c r="W32">
-        <v>-0.485540704138178</v>
-      </c>
       <c r="X32">
-        <v>-2.5875680790163</v>
+        <v>-0.485540704135921</v>
       </c>
       <c r="Y32">
-        <v>1.05616235065536</v>
+        <v>0.169151040081531</v>
       </c>
       <c r="Z32">
+        <v>1.04511848354637</v>
+      </c>
+      <c r="AA32">
         <v>0.0155906223665728</v>
       </c>
-      <c r="AA32">
-        <v>-0.590480977984785</v>
+      <c r="AB32">
+        <v>-0.269849018774391</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:28">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B33">
         <v>0.00881458966565349</v>
@@ -3257,7 +3356,7 @@
         <v>0.0490325490674652</v>
       </c>
       <c r="F33">
-        <v>0.0590153931426619</v>
+        <v>0.0588972518677869</v>
       </c>
       <c r="G33">
         <v>0.019935540928959</v>
@@ -3269,7 +3368,7 @@
         <v>0.326122897076721</v>
       </c>
       <c r="J33">
-        <v>0.149515347706408</v>
+        <v>0.149515347706406</v>
       </c>
       <c r="K33">
         <v>-0.2742315177481</v>
@@ -3284,10 +3383,10 @@
         <v>0.00224064601595518</v>
       </c>
       <c r="O33">
-        <v>5.45616399110618e-05</v>
+        <v>5.4561639911062e-05</v>
       </c>
       <c r="P33">
-        <v>-0.00014799139199548</v>
+        <v>-0.000147991391995479</v>
       </c>
       <c r="Q33">
         <v>0.001104704448038</v>
@@ -3302,30 +3401,33 @@
         <v>3.73164921749713</v>
       </c>
       <c r="U33">
+        <v>0.080780577260671</v>
+      </c>
+      <c r="V33">
         <v>3.35566144823923</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>0.913906824522309</v>
       </c>
-      <c r="W33">
-        <v>-0.730432509767316</v>
-      </c>
       <c r="X33">
-        <v>0.913687368325867</v>
+        <v>-0.730432509768249</v>
       </c>
       <c r="Y33">
-        <v>0.989825199424454</v>
+        <v>1.01902854360202</v>
       </c>
       <c r="Z33">
+        <v>0.97605788265735</v>
+      </c>
+      <c r="AA33">
         <v>0.0164239032884816</v>
       </c>
-      <c r="AA33">
-        <v>0.763038460876312</v>
+      <c r="AB33">
+        <v>0.492659962458387</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:28">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34">
         <v>0.0160364145658263</v>
@@ -3340,7 +3442,7 @@
         <v>0.0536597775812678</v>
       </c>
       <c r="F34">
-        <v>0.0465793288516832</v>
+        <v>0.0471854128935966</v>
       </c>
       <c r="G34">
         <v>0.0205393244868569</v>
@@ -3361,10 +3463,10 @@
         <v>0.207260554986778</v>
       </c>
       <c r="M34">
-        <v>0.027418504853362</v>
+        <v>0.0243641786623719</v>
       </c>
       <c r="N34">
-        <v>0.000763208462512595</v>
+        <v>0.00043595922776366</v>
       </c>
       <c r="O34">
         <v>-0.00258502863211183</v>
@@ -3373,42 +3475,45 @@
         <v>-0.00194560207195088</v>
       </c>
       <c r="Q34">
-        <v>-0.00085814043978589</v>
+        <v>-0.000585432744161776</v>
       </c>
       <c r="R34">
-        <v>0.0629422585013351</v>
+        <v>0.0586367029457796</v>
       </c>
       <c r="S34">
-        <v>0.023500701164744</v>
+        <v>0.0156106765345668</v>
       </c>
       <c r="T34">
-        <v>0.68083691022446</v>
+        <v>0.600751376639516</v>
       </c>
       <c r="U34">
+        <v>0.0866696892758589</v>
+      </c>
+      <c r="V34">
         <v>3.63654152113342</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <v>0.919118334403736</v>
       </c>
-      <c r="W34">
-        <v>1.41127049960005</v>
-      </c>
       <c r="X34">
-        <v>1.09501346185881</v>
+        <v>1.41127049960367</v>
       </c>
       <c r="Y34">
-        <v>0.963061159874462</v>
+        <v>-0.806273195866709</v>
       </c>
       <c r="Z34">
+        <v>0.930130573249988</v>
+      </c>
+      <c r="AA34">
         <v>0.0144777445925457</v>
       </c>
-      <c r="AA34">
-        <v>-0.0483531435235984</v>
+      <c r="AB34">
+        <v>-0.251024324986538</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:28">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B35">
         <v>0.0166390270867883</v>
@@ -3420,10 +3525,10 @@
         <v>0.0151856886949631</v>
       </c>
       <c r="E35">
-        <v>0.051802542937245</v>
+        <v>0.051607197841688</v>
       </c>
       <c r="F35">
-        <v>5.68157241573899e-05</v>
+        <v>-0.000569794671398363</v>
       </c>
       <c r="G35">
         <v>0.0151850748548865</v>
@@ -3444,10 +3549,10 @@
         <v>0.196205690769427</v>
       </c>
       <c r="M35">
-        <v>0.0269299883141363</v>
+        <v>0.027274744709592</v>
       </c>
       <c r="N35">
-        <v>-0.0056564294374281</v>
+        <v>-0.00544095669026831</v>
       </c>
       <c r="O35">
         <v>-0.000587970530368822</v>
@@ -3456,42 +3561,45 @@
         <v>-0.000302869893115774</v>
       </c>
       <c r="Q35">
-        <v>-0.00055977135142378</v>
+        <v>-0.000753696823867595</v>
       </c>
       <c r="R35">
-        <v>0.0631925417148788</v>
+        <v>0.0605587968589118</v>
       </c>
       <c r="S35">
-        <v>-0.133969537969895</v>
+        <v>-0.130197824299096</v>
       </c>
       <c r="T35">
-        <v>0.726206320225508</v>
+        <v>0.732330217969301</v>
       </c>
       <c r="U35">
+        <v>0.0757686800916731</v>
+      </c>
+      <c r="V35">
         <v>2.94392706621614</v>
       </c>
-      <c r="V35">
-        <v>0.931232742432658</v>
-      </c>
       <c r="W35">
-        <v>-0.824144253910764</v>
+        <v>0.931232742432657</v>
       </c>
       <c r="X35">
-        <v>0.121835458367477</v>
+        <v>-0.824144253915007</v>
       </c>
       <c r="Y35">
-        <v>0.968744140452917</v>
+        <v>0.0709358879754996</v>
       </c>
       <c r="Z35">
+        <v>1.00068258475361</v>
+      </c>
+      <c r="AA35">
         <v>0.0139078463835676</v>
       </c>
-      <c r="AA35">
-        <v>-0.423828515486821</v>
+      <c r="AB35">
+        <v>-0.27187804716895</v>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:28">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B36">
         <v>0.0129300524037366</v>
@@ -3503,10 +3611,10 @@
         <v>0.021406743785209</v>
       </c>
       <c r="E36">
-        <v>0.0515844976432836</v>
+        <v>0.0516106236237533</v>
       </c>
       <c r="F36">
-        <v>0.0215311173590645</v>
+        <v>0.0213491962539932</v>
       </c>
       <c r="G36">
         <v>0.021406743785209</v>
@@ -3518,7 +3626,7 @@
         <v>0.475553674381394</v>
       </c>
       <c r="J36">
-        <v>0.0618976942766494</v>
+        <v>0.061897694276649</v>
       </c>
       <c r="K36">
         <v>-0.272013123310375</v>
@@ -3533,7 +3641,7 @@
         <v>0.000680157082250581</v>
       </c>
       <c r="O36">
-        <v>-2.68470674871125e-05</v>
+        <v>-2.68470674871123e-05</v>
       </c>
       <c r="P36">
         <v>0.00043877427564367</v>
@@ -3551,30 +3659,33 @@
         <v>0.0982250877610291</v>
       </c>
       <c r="U36">
+        <v>0.0788197783758388</v>
+      </c>
+      <c r="V36">
         <v>4.37580469093585</v>
       </c>
-      <c r="V36">
+      <c r="W36">
         <v>0.923288431094891</v>
       </c>
-      <c r="W36">
-        <v>1.51776277387999</v>
-      </c>
       <c r="X36">
-        <v>-1.15232183184174</v>
+        <v>1.51776277389951</v>
       </c>
       <c r="Y36">
-        <v>1.10770841969219</v>
+        <v>0.469816271851209</v>
       </c>
       <c r="Z36">
+        <v>1.09515131021017</v>
+      </c>
+      <c r="AA36">
         <v>0.0159379240949826</v>
       </c>
-      <c r="AA36">
-        <v>0.281001650138757</v>
+      <c r="AB36">
+        <v>0.402306046776376</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:28">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B37">
         <v>0.019378683448207</v>
@@ -3586,10 +3697,10 @@
         <v>0.0127431254191818</v>
       </c>
       <c r="E37">
-        <v>0.0585702453224278</v>
+        <v>0.0587523318305125</v>
       </c>
       <c r="F37">
-        <v>0.00394883301773006</v>
+        <v>0.00423780389347218</v>
       </c>
       <c r="G37">
         <v>0.0127431254191818</v>
@@ -3631,33 +3742,36 @@
         <v>0.131534538093388</v>
       </c>
       <c r="T37">
-        <v>-1.97870344897175</v>
+        <v>-1.97870344897176</v>
       </c>
       <c r="U37">
+        <v>0.0649056543966191</v>
+      </c>
+      <c r="V37">
         <v>2.80416663950777</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <v>0.944826924421932</v>
       </c>
-      <c r="W37">
-        <v>0.709658773503338</v>
-      </c>
       <c r="X37">
-        <v>-0.801510330820907</v>
+        <v>0.709658773423918</v>
       </c>
       <c r="Y37">
-        <v>0.847050069997274</v>
+        <v>-0.523280947826687</v>
       </c>
       <c r="Z37">
+        <v>0.842820577380423</v>
+      </c>
+      <c r="AA37">
         <v>0.0145325579534586</v>
       </c>
-      <c r="AA37">
-        <v>-0.557419284141504</v>
+      <c r="AB37">
+        <v>-0.60042706829854</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:28">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B38">
         <v>0.0166122004357298</v>
@@ -3672,7 +3786,7 @@
         <v>0.0569694381534733</v>
       </c>
       <c r="F38">
-        <v>0.00239163901620455</v>
+        <v>0.00215853526195343</v>
       </c>
       <c r="G38">
         <v>0.0170477347931987</v>
@@ -3699,13 +3813,13 @@
         <v>0.00174168528289572</v>
       </c>
       <c r="O38">
-        <v>-3.86612272533335e-05</v>
+        <v>-3.86612272533332e-05</v>
       </c>
       <c r="P38">
-        <v>-8.19547140702226e-05</v>
+        <v>-8.19547140702227e-05</v>
       </c>
       <c r="Q38">
-        <v>0.000487221395101195</v>
+        <v>0.000487221395101196</v>
       </c>
       <c r="R38">
         <v>0.0804570072277418</v>
@@ -3717,30 +3831,33 @@
         <v>1.26271858356252</v>
       </c>
       <c r="U38">
+        <v>0.0720799883490948</v>
+      </c>
+      <c r="V38">
         <v>3.6031745715791</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <v>0.931874621662693</v>
       </c>
-      <c r="W38">
-        <v>-2.07262794079266</v>
-      </c>
       <c r="X38">
-        <v>0.566837583827508</v>
+        <v>-2.07262794073306</v>
       </c>
       <c r="Y38">
-        <v>1.0703991782136</v>
+        <v>-0.643497018984827</v>
       </c>
       <c r="Z38">
+        <v>1.07901967771439</v>
+      </c>
+      <c r="AA38">
         <v>0.0165550813212645</v>
       </c>
-      <c r="AA38">
-        <v>0.455274433787522</v>
+      <c r="AB38">
+        <v>0.271741926045975</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:28">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B39">
         <v>0.0117889773062187</v>
@@ -3752,10 +3869,10 @@
         <v>0.0226879140854845</v>
       </c>
       <c r="E39">
-        <v>0.0652925068842347</v>
+        <v>0.0652925068842345</v>
       </c>
       <c r="F39">
-        <v>0.0742138020614793</v>
+        <v>0.0740091211179942</v>
       </c>
       <c r="G39">
         <v>0.0226879947965239</v>
@@ -3767,7 +3884,7 @@
         <v>0.404298244043134</v>
       </c>
       <c r="J39">
-        <v>0.0768814325141799</v>
+        <v>0.0768814325141816</v>
       </c>
       <c r="K39">
         <v>-0.26293492117317</v>
@@ -3776,54 +3893,57 @@
         <v>0.216701782541297</v>
       </c>
       <c r="M39">
-        <v>0.037144810837062</v>
+        <v>0.0395545356425769</v>
       </c>
       <c r="N39">
-        <v>0.00046086764986979</v>
+        <v>-5.55019513119675e-05</v>
       </c>
       <c r="O39">
-        <v>-6.20510290493012e-06</v>
+        <v>-6.20510290493006e-06</v>
       </c>
       <c r="P39">
-        <v>-0.000420203268863843</v>
+        <v>-0.000420203268863842</v>
       </c>
       <c r="Q39">
-        <v>-0.00317413729926709</v>
+        <v>-0.000707038093620926</v>
       </c>
       <c r="R39">
-        <v>0.0474981740539727</v>
+        <v>0.0472790199886648</v>
       </c>
       <c r="S39">
-        <v>0.0256340039517877</v>
+        <v>0.0017139486658735</v>
       </c>
       <c r="T39">
-        <v>0.912287191551589</v>
+        <v>0.973986507239334</v>
       </c>
       <c r="U39">
+        <v>0.0892079950258481</v>
+      </c>
+      <c r="V39">
         <v>3.68945821315586</v>
       </c>
-      <c r="V39">
+      <c r="W39">
         <v>0.920027684349608</v>
       </c>
-      <c r="W39">
-        <v>-0.400862997033865</v>
-      </c>
       <c r="X39">
-        <v>0.48768383003101</v>
+        <v>-0.400862997033977</v>
       </c>
       <c r="Y39">
-        <v>1.06547540132603</v>
+        <v>-2.46286352944378</v>
       </c>
       <c r="Z39">
+        <v>1.02972252463104</v>
+      </c>
+      <c r="AA39">
         <v>0.0174159070567434</v>
       </c>
-      <c r="AA39">
-        <v>0.175574785184368</v>
+      <c r="AB39">
+        <v>-0.0724465180988842</v>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:28">
       <c r="A40" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B40">
         <v>0.018018018018018</v>
@@ -3835,10 +3955,10 @@
         <v>0.0226640318604604</v>
       </c>
       <c r="E40">
-        <v>0.0555953126232959</v>
+        <v>0.055595312623296</v>
       </c>
       <c r="F40">
-        <v>0.0423586679624272</v>
+        <v>0.0423586679624271</v>
       </c>
       <c r="G40">
         <v>0.0226643468607754</v>
@@ -3859,54 +3979,57 @@
         <v>0.215427630100461</v>
       </c>
       <c r="M40">
-        <v>0.0596429941227705</v>
+        <v>0.0618970067090514</v>
       </c>
       <c r="N40">
-        <v>0.000409366180251967</v>
+        <v>0.00147376101266241</v>
       </c>
       <c r="O40">
-        <v>0.000239927956350057</v>
+        <v>0.000239927956350058</v>
       </c>
       <c r="P40">
-        <v>-0.000158971182373318</v>
+        <v>-0.000158971182373319</v>
       </c>
       <c r="Q40">
-        <v>-0.000529648379374242</v>
+        <v>0.000691275104861267</v>
       </c>
       <c r="R40">
-        <v>0.063810180310566</v>
+        <v>0.0636507415350558</v>
       </c>
       <c r="S40">
-        <v>0.0186704434362845</v>
+        <v>0.0420750480303614</v>
       </c>
       <c r="T40">
-        <v>1.41840504112023</v>
+        <v>1.47307686000038</v>
       </c>
       <c r="U40">
+        <v>0.0919408776129426</v>
+      </c>
+      <c r="V40">
         <v>4.46947547692328</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>0.909879266755755</v>
       </c>
-      <c r="W40">
-        <v>1.2102469506713</v>
-      </c>
       <c r="X40">
-        <v>-0.587404322954513</v>
+        <v>1.21024695067678</v>
       </c>
       <c r="Y40">
-        <v>0.939497303142611</v>
+        <v>0.613836418511513</v>
       </c>
       <c r="Z40">
+        <v>0.973687312197382</v>
+      </c>
+      <c r="AA40">
         <v>0.0146197522283737</v>
       </c>
-      <c r="AA40">
-        <v>0.172025904277018</v>
+      <c r="AB40">
+        <v>0.548442992474778</v>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:28">
       <c r="A41" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B41">
         <v>0.0218181818181818</v>
@@ -3918,10 +4041,10 @@
         <v>0.022487502466666</v>
       </c>
       <c r="E41">
-        <v>0.065612318978133</v>
+        <v>0.0647809966361824</v>
       </c>
       <c r="F41">
-        <v>0.0465857645278992</v>
+        <v>0.0469341559959676</v>
       </c>
       <c r="G41">
         <v>0.0222972371254013</v>
@@ -3933,7 +4056,7 @@
         <v>0.37828465028424</v>
       </c>
       <c r="J41">
-        <v>0.048675410971366</v>
+        <v>0.0486754109713569</v>
       </c>
       <c r="K41">
         <v>-0.253422772445006</v>
@@ -3942,54 +4065,57 @@
         <v>0.224137553578769</v>
       </c>
       <c r="M41">
-        <v>0.0429072280317572</v>
+        <v>0.0498187318696548</v>
       </c>
       <c r="N41">
-        <v>-0.00416716951724084</v>
+        <v>-0.00306761208848441</v>
       </c>
       <c r="O41">
-        <v>-7.92764686140063e-05</v>
+        <v>-7.92764686140065e-05</v>
       </c>
       <c r="P41">
-        <v>4.74055136622706e-05</v>
+        <v>4.740551366227e-05</v>
       </c>
       <c r="Q41">
-        <v>0.0042877706687894</v>
+        <v>0.00275624425016438</v>
       </c>
       <c r="R41">
-        <v>0.0826971388201054</v>
+        <v>0.0782971388201054</v>
       </c>
       <c r="S41">
-        <v>-0.0728663787556849</v>
+        <v>-0.0650253518753237</v>
       </c>
       <c r="T41">
-        <v>0.933459988123445</v>
+        <v>1.08683881122938</v>
       </c>
       <c r="U41">
-        <v>4.6916762392681</v>
+        <v>0.098529645738086</v>
       </c>
       <c r="V41">
+        <v>4.69167623926808</v>
+      </c>
+      <c r="W41">
         <v>0.926206485054065</v>
       </c>
-      <c r="W41">
-        <v>-0.787205708643641</v>
-      </c>
       <c r="X41">
-        <v>-1.69455934132459</v>
+        <v>-0.787205708647987</v>
       </c>
       <c r="Y41">
-        <v>1.02138039698852</v>
+        <v>2.67395480975762</v>
       </c>
       <c r="Z41">
+        <v>1.02465332993941</v>
+      </c>
+      <c r="AA41">
         <v>0.0157797226669743</v>
       </c>
-      <c r="AA41">
-        <v>-0.354922469674246</v>
+      <c r="AB41">
+        <v>-0.00648323904881874</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:28">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B42">
         <v>0.0493951612903226</v>
@@ -4031,7 +4157,7 @@
         <v>-0.00626678893930677</v>
       </c>
       <c r="O42">
-        <v>0.000227178473585469</v>
+        <v>0.000227178473585468</v>
       </c>
       <c r="P42">
         <v>0.00358401713339298</v>
@@ -4049,30 +4175,33 @@
         <v>1.827190671876</v>
       </c>
       <c r="U42">
-        <v>4.15966253816412</v>
+        <v>0.246777354846434</v>
       </c>
       <c r="V42">
+        <v>4.1596625381641</v>
+      </c>
+      <c r="W42">
         <v>0.874617590281242</v>
       </c>
-      <c r="W42">
-        <v>-0.449599716257388</v>
-      </c>
       <c r="X42">
-        <v>-0.480404067142626</v>
+        <v>-0.449599716258327</v>
       </c>
       <c r="Y42">
-        <v>0.67358089270154</v>
+        <v>-0.499105624220215</v>
       </c>
       <c r="Z42">
+        <v>0.538755140050969</v>
+      </c>
+      <c r="AA42">
         <v>0.00944419553063511</v>
       </c>
-      <c r="AA42">
-        <v>0.2746462865345</v>
+      <c r="AB42">
+        <v>-0.214174092337781</v>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:28">
       <c r="A43" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B43">
         <v>0.2</v>
@@ -4084,7 +4213,7 @@
         <v>0.05</v>
       </c>
       <c r="E43">
-        <v>0.306718767791671</v>
+        <v>0.248877593896021</v>
       </c>
       <c r="F43">
         <v>0.277665759407482</v>
@@ -4114,7 +4243,7 @@
         <v>0.0116042004087977</v>
       </c>
       <c r="O43">
-        <v>-0.00176149037799115</v>
+        <v>-0.00176149037799114</v>
       </c>
       <c r="P43">
         <v>-0.0359473599965106</v>
@@ -4132,30 +4261,33 @@
         <v>0.882645993666084</v>
       </c>
       <c r="U43">
+        <v>1.03215578066265</v>
+      </c>
+      <c r="V43">
         <v>1.01020408163265</v>
       </c>
-      <c r="V43">
+      <c r="W43">
         <v>0.78344949004277</v>
       </c>
-      <c r="W43">
-        <v>-1.72972907025383</v>
-      </c>
       <c r="X43">
-        <v>-2.20627013906616</v>
+        <v>-1.72972907025385</v>
       </c>
       <c r="Y43">
-        <v>0.316045913814248</v>
+        <v>-1.04758760991732</v>
       </c>
       <c r="Z43">
+        <v>0.39517721302673</v>
+      </c>
+      <c r="AA43">
         <v>0.00642756742316938</v>
       </c>
-      <c r="AA43">
-        <v>-0.760420169006862</v>
+      <c r="AB43">
+        <v>-0.497965332827767</v>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:28">
       <c r="A44" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B44">
         <v>0.106617647058824</v>
@@ -4167,7 +4299,7 @@
         <v>0.0941176470588235</v>
       </c>
       <c r="E44">
-        <v>0.17223487960862</v>
+        <v>0.168015456926592</v>
       </c>
       <c r="F44">
         <v>0.212197700127084</v>
@@ -4197,10 +4329,10 @@
         <v>0.0135902114777562</v>
       </c>
       <c r="O44">
-        <v>0.00233196065075343</v>
+        <v>0.00233196065075344</v>
       </c>
       <c r="P44">
-        <v>-0.000960797160877371</v>
+        <v>-0.000960797160877369</v>
       </c>
       <c r="Q44">
         <v>-0.0115355589788568</v>
@@ -4209,36 +4341,39 @@
         <v>0.147931491129832</v>
       </c>
       <c r="S44">
-        <v>0.0999214999530457</v>
+        <v>0.0999214999530456</v>
       </c>
       <c r="T44">
         <v>2.19642155352231</v>
       </c>
       <c r="U44">
+        <v>0.424083294584985</v>
+      </c>
+      <c r="V44">
         <v>3.21537487788863</v>
       </c>
-      <c r="V44">
+      <c r="W44">
         <v>0.90539233240597</v>
       </c>
-      <c r="W44">
-        <v>0.292188771086001</v>
-      </c>
       <c r="X44">
-        <v>1.25358684555304</v>
+        <v>0.292188771086005</v>
       </c>
       <c r="Y44">
-        <v>1.88897245302525</v>
+        <v>0.749435981204181</v>
       </c>
       <c r="Z44">
+        <v>1.76758460053992</v>
+      </c>
+      <c r="AA44">
         <v>0.00861579736784824</v>
       </c>
-      <c r="AA44">
-        <v>0.836037129462003</v>
+      <c r="AB44">
+        <v>0.646504676850528</v>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:28">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B45">
         <v>0.357142857142857</v>
@@ -4298,25 +4433,28 @@
         <v>3.13746084020405</v>
       </c>
       <c r="U45">
+        <v>0.881356348849824</v>
+      </c>
+      <c r="V45">
         <v>1.75897892732976</v>
       </c>
-      <c r="V45">
+      <c r="W45">
         <v>0.874853617732142</v>
       </c>
-      <c r="W45">
-        <v>0.303596422697832</v>
-      </c>
       <c r="X45">
-        <v>-0.854212213859845</v>
+        <v>0.303596422697829</v>
       </c>
       <c r="Y45">
-        <v>0.692824659123163</v>
+        <v>-0.7268984969884</v>
       </c>
       <c r="Z45">
+        <v>0.736775497724834</v>
+      </c>
+      <c r="AA45">
         <v>0.0133162403328807</v>
       </c>
-      <c r="AA45">
-        <v>-0.187871788619365</v>
+      <c r="AB45">
+        <v>-0.0849423414531283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>